<commit_message>
Fixes for #422: Added model for xform to catch entire submitted survey response. - Also improved error messaging, but determined that it's not possible to customize error messages in GeoODK Collect - Includes some of brian's work for 440 (sorry brian)
</commit_message>
<xml_diff>
--- a/cadasta/questionnaires/tests/files/test_standard_questionnaire_2.xlsx
+++ b/cadasta/questionnaires/tests/files/test_standard_questionnaire_2.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="191">
   <si>
     <t>type</t>
   </si>
@@ -107,15 +107,36 @@
     <t>Party Name</t>
   </si>
   <si>
+    <t>select_one geotype</t>
+  </si>
+  <si>
+    <t>location_choice</t>
+  </si>
+  <si>
+    <t>Geoshape or Geotrace?</t>
+  </si>
+  <si>
     <t>geoshape</t>
   </si>
   <si>
-    <t>location_geometry</t>
+    <t>location_geoshape</t>
   </si>
   <si>
     <t>Location of Parcel</t>
   </si>
   <si>
+    <t>${geotype}='geoshape'</t>
+  </si>
+  <si>
+    <t>geotrace</t>
+  </si>
+  <si>
+    <t>location_geotrace</t>
+  </si>
+  <si>
+    <t>${geotype}=‘geotrace'</t>
+  </si>
+  <si>
     <t>select_one land_type</t>
   </si>
   <si>
@@ -570,6 +591,15 @@
   </si>
   <si>
     <t>Female</t>
+  </si>
+  <si>
+    <t>geotype</t>
+  </si>
+  <si>
+    <t>Geoshape</t>
+  </si>
+  <si>
+    <t>Geotrace</t>
   </si>
   <si>
     <t>form_id</t>
@@ -673,7 +703,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="42">
+  <borders count="40">
     <border>
       <left/>
       <right/>
@@ -750,30 +780,6 @@
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="9"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1148,7 +1154,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1194,33 +1200,33 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1233,139 +1239,133 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="36" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="37" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="38" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="3" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="3" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="3" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="38" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="39" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2477,7 +2477,7 @@
     <col min="6" max="6" width="16.3516" style="1" customWidth="1"/>
     <col min="7" max="7" width="16.3516" style="1" customWidth="1"/>
     <col min="8" max="8" width="16.3516" style="1" customWidth="1"/>
-    <col min="9" max="9" width="16.3516" style="1" customWidth="1"/>
+    <col min="9" max="9" width="29.2422" style="1" customWidth="1"/>
     <col min="10" max="10" width="16.3516" style="1" customWidth="1"/>
     <col min="11" max="11" width="16.3516" style="1" customWidth="1"/>
     <col min="12" max="12" width="16.3516" style="1" customWidth="1"/>
@@ -2735,15 +2735,21 @@
       <c r="N12" s="12"/>
     </row>
     <row r="13" ht="13.5" customHeight="1">
-      <c r="A13" s="13"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
+      <c r="A13" t="s" s="7">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s" s="8">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s" s="7">
+        <v>25</v>
+      </c>
+      <c r="D13" s="9"/>
       <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
       <c r="J13" s="10"/>
       <c r="K13" s="11"/>
       <c r="L13" s="11"/>
@@ -2751,16 +2757,24 @@
       <c r="N13" s="12"/>
     </row>
     <row r="14" ht="13.5" customHeight="1">
-      <c r="A14" s="15"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="11"/>
+      <c r="A14" t="s" s="7">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s" s="7">
+        <v>28</v>
+      </c>
+      <c r="D14" s="9"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" t="s" s="15">
+        <v>29</v>
+      </c>
+      <c r="J14" s="10"/>
       <c r="K14" s="11"/>
       <c r="L14" s="11"/>
       <c r="M14" s="11"/>
@@ -2768,20 +2782,22 @@
     </row>
     <row r="15" ht="13.5" customHeight="1">
       <c r="A15" t="s" s="7">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s" s="8">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s" s="7">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="13"/>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
+      <c r="I15" t="s" s="15">
+        <v>32</v>
+      </c>
       <c r="J15" s="10"/>
       <c r="K15" s="11"/>
       <c r="L15" s="11"/>
@@ -2790,13 +2806,13 @@
     </row>
     <row r="16" ht="24.75" customHeight="1">
       <c r="A16" t="s" s="7">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B16" t="s" s="8">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C16" t="s" s="7">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="D16" s="13"/>
       <c r="E16" t="s" s="7">
@@ -2830,13 +2846,13 @@
     </row>
     <row r="18" ht="13.5" customHeight="1">
       <c r="A18" t="s" s="7">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B18" t="s" s="8">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C18" t="s" s="7">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
@@ -2852,13 +2868,13 @@
     </row>
     <row r="19" ht="13.5" customHeight="1">
       <c r="A19" t="s" s="7">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B19" t="s" s="8">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C19" t="s" s="7">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
@@ -2890,13 +2906,13 @@
     </row>
     <row r="21" ht="24.75" customHeight="1">
       <c r="A21" t="s" s="7">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B21" t="s" s="8">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C21" t="s" s="7">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="D21" s="13"/>
       <c r="E21" t="s" s="7">
@@ -2913,15 +2929,15 @@
       <c r="N21" s="12"/>
     </row>
     <row r="22" ht="18" customHeight="1">
-      <c r="A22" s="17"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
+      <c r="A22" s="16"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
       <c r="J22" s="10"/>
       <c r="K22" s="11"/>
       <c r="L22" s="11"/>
@@ -2930,13 +2946,13 @@
     </row>
     <row r="23" ht="13.5" customHeight="1">
       <c r="A23" t="s" s="7">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="B23" t="s" s="7">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C23" t="s" s="7">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="D23" s="13"/>
       <c r="E23" s="13"/>
@@ -2958,14 +2974,14 @@
         <v>1</v>
       </c>
       <c r="C24" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="19"/>
+        <v>47</v>
+      </c>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
       <c r="J24" s="10"/>
       <c r="K24" s="11"/>
       <c r="L24" s="11"/>
@@ -2974,24 +2990,24 @@
     </row>
     <row r="25" ht="24.75" customHeight="1">
       <c r="A25" t="s" s="2">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C25" t="s" s="2">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="D25" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
+        <v>51</v>
+      </c>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
       <c r="H25" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="I25" s="19"/>
+        <v>52</v>
+      </c>
+      <c r="I25" s="18"/>
       <c r="J25" s="10"/>
       <c r="K25" s="11"/>
       <c r="L25" s="11"/>
@@ -3000,22 +3016,22 @@
     </row>
     <row r="26" ht="24.75" customHeight="1">
       <c r="A26" t="s" s="2">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C26" t="s" s="2">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="D26" s="2"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
       <c r="H26" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="I26" s="19"/>
+        <v>56</v>
+      </c>
+      <c r="I26" s="18"/>
       <c r="J26" s="10"/>
       <c r="K26" s="11"/>
       <c r="L26" s="11"/>
@@ -3024,22 +3040,22 @@
     </row>
     <row r="27" ht="24.75" customHeight="1">
       <c r="A27" t="s" s="2">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C27" t="s" s="2">
+        <v>59</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" t="s" s="2">
         <v>52</v>
       </c>
-      <c r="D27" s="2"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
-      <c r="H27" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="I27" s="19"/>
+      <c r="I27" s="18"/>
       <c r="J27" s="10"/>
       <c r="K27" s="11"/>
       <c r="L27" s="11"/>
@@ -3051,19 +3067,19 @@
         <v>20</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="C28" t="s" s="2">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="D28" t="s" s="2">
-        <v>55</v>
-      </c>
-      <c r="E28" s="19"/>
+        <v>62</v>
+      </c>
+      <c r="E28" s="18"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
       <c r="J28" s="10"/>
       <c r="K28" s="11"/>
       <c r="L28" s="11"/>
@@ -3072,7 +3088,7 @@
     </row>
     <row r="29" ht="13.5" customHeight="1">
       <c r="A29" t="s" s="7">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="B29" s="13"/>
       <c r="C29" s="13"/>
@@ -3089,15 +3105,15 @@
       <c r="N29" s="12"/>
     </row>
     <row r="30" ht="13.5" customHeight="1">
-      <c r="A30" s="17"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="18"/>
-      <c r="I30" s="18"/>
+      <c r="A30" s="16"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="17"/>
       <c r="J30" s="10"/>
       <c r="K30" s="11"/>
       <c r="L30" s="11"/>
@@ -3105,21 +3121,21 @@
       <c r="N30" s="12"/>
     </row>
     <row r="31" ht="13.5" customHeight="1">
-      <c r="A31" t="s" s="20">
-        <v>37</v>
-      </c>
-      <c r="B31" t="s" s="20">
-        <v>57</v>
-      </c>
-      <c r="C31" t="s" s="20">
-        <v>58</v>
-      </c>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21"/>
-      <c r="I31" s="21"/>
+      <c r="A31" t="s" s="15">
+        <v>44</v>
+      </c>
+      <c r="B31" t="s" s="15">
+        <v>64</v>
+      </c>
+      <c r="C31" t="s" s="15">
+        <v>65</v>
+      </c>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="19"/>
       <c r="J31" s="10"/>
       <c r="K31" s="11"/>
       <c r="L31" s="11"/>
@@ -3127,21 +3143,21 @@
       <c r="N31" s="12"/>
     </row>
     <row r="32" ht="24.75" customHeight="1">
-      <c r="A32" t="s" s="22">
+      <c r="A32" t="s" s="20">
         <v>20</v>
       </c>
-      <c r="B32" t="s" s="22">
-        <v>53</v>
-      </c>
-      <c r="C32" t="s" s="22">
-        <v>54</v>
-      </c>
-      <c r="D32" s="23"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="23"/>
-      <c r="H32" s="23"/>
-      <c r="I32" s="23"/>
+      <c r="B32" t="s" s="20">
+        <v>60</v>
+      </c>
+      <c r="C32" t="s" s="20">
+        <v>61</v>
+      </c>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="21"/>
       <c r="J32" s="10"/>
       <c r="K32" s="11"/>
       <c r="L32" s="11"/>
@@ -3149,17 +3165,17 @@
       <c r="N32" s="12"/>
     </row>
     <row r="33" ht="24.75" customHeight="1">
-      <c r="A33" t="s" s="20">
-        <v>56</v>
-      </c>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="21"/>
-      <c r="I33" s="21"/>
+      <c r="A33" t="s" s="15">
+        <v>63</v>
+      </c>
+      <c r="B33" s="19"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="19"/>
       <c r="J33" s="10"/>
       <c r="K33" s="11"/>
       <c r="L33" s="11"/>
@@ -3167,15 +3183,15 @@
       <c r="N33" s="12"/>
     </row>
     <row r="34" ht="24.75" customHeight="1">
-      <c r="A34" s="17"/>
-      <c r="B34" s="17"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
-      <c r="H34" s="18"/>
-      <c r="I34" s="18"/>
+      <c r="A34" s="16"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="17"/>
       <c r="J34" s="10"/>
       <c r="K34" s="11"/>
       <c r="L34" s="11"/>
@@ -3183,22 +3199,22 @@
       <c r="N34" s="12"/>
     </row>
     <row r="35" ht="13.5" customHeight="1">
-      <c r="A35" t="s" s="20">
-        <v>37</v>
-      </c>
-      <c r="B35" t="s" s="20">
-        <v>59</v>
-      </c>
-      <c r="C35" t="s" s="20">
-        <v>60</v>
-      </c>
-      <c r="D35" s="21"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="21"/>
-      <c r="H35" s="21"/>
-      <c r="I35" t="s" s="20">
-        <v>61</v>
+      <c r="A35" t="s" s="15">
+        <v>44</v>
+      </c>
+      <c r="B35" t="s" s="15">
+        <v>66</v>
+      </c>
+      <c r="C35" t="s" s="15">
+        <v>67</v>
+      </c>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="19"/>
+      <c r="I35" t="s" s="15">
+        <v>68</v>
       </c>
       <c r="J35" s="10"/>
       <c r="K35" s="11"/>
@@ -3207,23 +3223,23 @@
       <c r="N35" s="12"/>
     </row>
     <row r="36" ht="13.5" customHeight="1">
-      <c r="A36" t="s" s="22">
-        <v>62</v>
-      </c>
-      <c r="B36" t="s" s="22">
-        <v>63</v>
-      </c>
-      <c r="C36" t="s" s="22">
-        <v>64</v>
-      </c>
-      <c r="D36" s="23"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
-      <c r="G36" s="23"/>
-      <c r="H36" t="s" s="22">
-        <v>65</v>
-      </c>
-      <c r="I36" s="23"/>
+      <c r="A36" t="s" s="20">
+        <v>69</v>
+      </c>
+      <c r="B36" t="s" s="20">
+        <v>70</v>
+      </c>
+      <c r="C36" t="s" s="20">
+        <v>71</v>
+      </c>
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="21"/>
+      <c r="H36" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="I36" s="21"/>
       <c r="J36" s="10"/>
       <c r="K36" s="11"/>
       <c r="L36" s="11"/>
@@ -3231,25 +3247,25 @@
       <c r="N36" s="12"/>
     </row>
     <row r="37" ht="13.5" customHeight="1">
-      <c r="A37" t="s" s="22">
-        <v>66</v>
-      </c>
-      <c r="B37" t="s" s="22">
-        <v>67</v>
-      </c>
-      <c r="C37" t="s" s="22">
-        <v>68</v>
-      </c>
-      <c r="D37" t="s" s="22">
-        <v>69</v>
-      </c>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
-      <c r="G37" s="23"/>
-      <c r="H37" t="s" s="22">
-        <v>70</v>
-      </c>
-      <c r="I37" s="23"/>
+      <c r="A37" t="s" s="20">
+        <v>73</v>
+      </c>
+      <c r="B37" t="s" s="20">
+        <v>74</v>
+      </c>
+      <c r="C37" t="s" s="20">
+        <v>75</v>
+      </c>
+      <c r="D37" t="s" s="20">
+        <v>76</v>
+      </c>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="21"/>
+      <c r="H37" t="s" s="20">
+        <v>77</v>
+      </c>
+      <c r="I37" s="21"/>
       <c r="J37" s="10"/>
       <c r="K37" s="11"/>
       <c r="L37" s="11"/>
@@ -3257,21 +3273,21 @@
       <c r="N37" s="12"/>
     </row>
     <row r="38" ht="13.5" customHeight="1">
-      <c r="A38" t="s" s="22">
-        <v>50</v>
-      </c>
-      <c r="B38" t="s" s="22">
-        <v>71</v>
-      </c>
-      <c r="C38" t="s" s="22">
-        <v>72</v>
-      </c>
-      <c r="D38" s="23"/>
-      <c r="E38" s="23"/>
-      <c r="F38" s="23"/>
-      <c r="G38" s="23"/>
-      <c r="H38" s="23"/>
-      <c r="I38" s="23"/>
+      <c r="A38" t="s" s="20">
+        <v>57</v>
+      </c>
+      <c r="B38" t="s" s="20">
+        <v>78</v>
+      </c>
+      <c r="C38" t="s" s="20">
+        <v>79</v>
+      </c>
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="21"/>
       <c r="J38" s="10"/>
       <c r="K38" s="11"/>
       <c r="L38" s="11"/>
@@ -3279,17 +3295,17 @@
       <c r="N38" s="12"/>
     </row>
     <row r="39" ht="13.5" customHeight="1">
-      <c r="A39" t="s" s="20">
-        <v>56</v>
-      </c>
-      <c r="B39" s="21"/>
-      <c r="C39" s="21"/>
-      <c r="D39" s="21"/>
-      <c r="E39" s="21"/>
-      <c r="F39" s="21"/>
-      <c r="G39" s="21"/>
-      <c r="H39" s="21"/>
-      <c r="I39" s="21"/>
+      <c r="A39" t="s" s="15">
+        <v>63</v>
+      </c>
+      <c r="B39" s="19"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="19"/>
+      <c r="I39" s="19"/>
       <c r="J39" s="10"/>
       <c r="K39" s="11"/>
       <c r="L39" s="11"/>
@@ -3297,15 +3313,15 @@
       <c r="N39" s="12"/>
     </row>
     <row r="40" ht="13.5" customHeight="1">
-      <c r="A40" s="17"/>
-      <c r="B40" s="17"/>
-      <c r="C40" s="17"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="18"/>
-      <c r="I40" s="18"/>
+      <c r="A40" s="16"/>
+      <c r="B40" s="16"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="17"/>
+      <c r="H40" s="17"/>
+      <c r="I40" s="17"/>
       <c r="J40" s="10"/>
       <c r="K40" s="11"/>
       <c r="L40" s="11"/>
@@ -3313,22 +3329,22 @@
       <c r="N40" s="12"/>
     </row>
     <row r="41" ht="13.5" customHeight="1">
-      <c r="A41" t="s" s="20">
-        <v>37</v>
-      </c>
-      <c r="B41" t="s" s="20">
-        <v>73</v>
-      </c>
-      <c r="C41" t="s" s="20">
-        <v>74</v>
-      </c>
-      <c r="D41" s="21"/>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21"/>
-      <c r="G41" s="21"/>
-      <c r="H41" s="21"/>
-      <c r="I41" t="s" s="20">
-        <v>75</v>
+      <c r="A41" t="s" s="15">
+        <v>44</v>
+      </c>
+      <c r="B41" t="s" s="15">
+        <v>80</v>
+      </c>
+      <c r="C41" t="s" s="15">
+        <v>81</v>
+      </c>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="19"/>
+      <c r="I41" t="s" s="15">
+        <v>82</v>
       </c>
       <c r="J41" s="10"/>
       <c r="K41" s="11"/>
@@ -3337,21 +3353,21 @@
       <c r="N41" s="12"/>
     </row>
     <row r="42" ht="13.5" customHeight="1">
-      <c r="A42" t="s" s="22">
-        <v>76</v>
-      </c>
-      <c r="B42" t="s" s="22">
-        <v>77</v>
-      </c>
-      <c r="C42" t="s" s="22">
-        <v>78</v>
-      </c>
-      <c r="D42" s="23"/>
-      <c r="E42" s="23"/>
-      <c r="F42" s="23"/>
-      <c r="G42" s="23"/>
-      <c r="H42" s="23"/>
-      <c r="I42" s="23"/>
+      <c r="A42" t="s" s="20">
+        <v>83</v>
+      </c>
+      <c r="B42" t="s" s="20">
+        <v>84</v>
+      </c>
+      <c r="C42" t="s" s="20">
+        <v>85</v>
+      </c>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="21"/>
+      <c r="H42" s="21"/>
+      <c r="I42" s="21"/>
       <c r="J42" s="10"/>
       <c r="K42" s="11"/>
       <c r="L42" s="11"/>
@@ -3359,21 +3375,21 @@
       <c r="N42" s="12"/>
     </row>
     <row r="43" ht="13.5" customHeight="1">
-      <c r="A43" t="s" s="22">
-        <v>50</v>
-      </c>
-      <c r="B43" t="s" s="22">
-        <v>79</v>
-      </c>
-      <c r="C43" t="s" s="22">
-        <v>80</v>
-      </c>
-      <c r="D43" s="23"/>
-      <c r="E43" s="23"/>
-      <c r="F43" s="23"/>
-      <c r="G43" s="23"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
+      <c r="A43" t="s" s="20">
+        <v>57</v>
+      </c>
+      <c r="B43" t="s" s="20">
+        <v>86</v>
+      </c>
+      <c r="C43" t="s" s="20">
+        <v>87</v>
+      </c>
+      <c r="D43" s="21"/>
+      <c r="E43" s="21"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="21"/>
+      <c r="H43" s="21"/>
+      <c r="I43" s="21"/>
       <c r="J43" s="10"/>
       <c r="K43" s="11"/>
       <c r="L43" s="11"/>
@@ -3381,17 +3397,17 @@
       <c r="N43" s="12"/>
     </row>
     <row r="44" ht="24.75" customHeight="1">
-      <c r="A44" t="s" s="20">
-        <v>56</v>
-      </c>
-      <c r="B44" s="21"/>
-      <c r="C44" s="21"/>
-      <c r="D44" s="21"/>
-      <c r="E44" s="21"/>
-      <c r="F44" s="21"/>
-      <c r="G44" s="21"/>
-      <c r="H44" s="21"/>
-      <c r="I44" s="21"/>
+      <c r="A44" t="s" s="15">
+        <v>63</v>
+      </c>
+      <c r="B44" s="19"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="19"/>
+      <c r="I44" s="19"/>
       <c r="J44" s="10"/>
       <c r="K44" s="11"/>
       <c r="L44" s="11"/>
@@ -3399,15 +3415,15 @@
       <c r="N44" s="12"/>
     </row>
     <row r="45" ht="13.5" customHeight="1">
-      <c r="A45" s="17"/>
-      <c r="B45" s="17"/>
-      <c r="C45" s="17"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="18"/>
-      <c r="G45" s="18"/>
-      <c r="H45" s="18"/>
-      <c r="I45" s="18"/>
+      <c r="A45" s="16"/>
+      <c r="B45" s="16"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="17"/>
+      <c r="F45" s="17"/>
+      <c r="G45" s="17"/>
+      <c r="H45" s="17"/>
+      <c r="I45" s="17"/>
       <c r="J45" s="10"/>
       <c r="K45" s="11"/>
       <c r="L45" s="11"/>
@@ -3415,21 +3431,21 @@
       <c r="N45" s="12"/>
     </row>
     <row r="46" ht="13.5" customHeight="1">
-      <c r="A46" t="s" s="20">
-        <v>37</v>
-      </c>
-      <c r="B46" t="s" s="20">
-        <v>81</v>
-      </c>
-      <c r="C46" t="s" s="20">
-        <v>82</v>
-      </c>
-      <c r="D46" s="21"/>
-      <c r="E46" s="21"/>
-      <c r="F46" s="21"/>
-      <c r="G46" s="21"/>
-      <c r="H46" s="21"/>
-      <c r="I46" s="21"/>
+      <c r="A46" t="s" s="15">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s" s="15">
+        <v>88</v>
+      </c>
+      <c r="C46" t="s" s="15">
+        <v>89</v>
+      </c>
+      <c r="D46" s="19"/>
+      <c r="E46" s="19"/>
+      <c r="F46" s="19"/>
+      <c r="G46" s="19"/>
+      <c r="H46" s="19"/>
+      <c r="I46" s="19"/>
       <c r="J46" s="10"/>
       <c r="K46" s="11"/>
       <c r="L46" s="11"/>
@@ -3437,21 +3453,21 @@
       <c r="N46" s="12"/>
     </row>
     <row r="47" ht="13.5" customHeight="1">
-      <c r="A47" t="s" s="22">
+      <c r="A47" t="s" s="20">
         <v>20</v>
       </c>
-      <c r="B47" t="s" s="22">
-        <v>53</v>
-      </c>
-      <c r="C47" t="s" s="22">
-        <v>54</v>
-      </c>
-      <c r="D47" s="23"/>
-      <c r="E47" s="23"/>
-      <c r="F47" s="23"/>
-      <c r="G47" s="23"/>
-      <c r="H47" s="23"/>
-      <c r="I47" s="23"/>
+      <c r="B47" t="s" s="20">
+        <v>60</v>
+      </c>
+      <c r="C47" t="s" s="20">
+        <v>61</v>
+      </c>
+      <c r="D47" s="21"/>
+      <c r="E47" s="21"/>
+      <c r="F47" s="21"/>
+      <c r="G47" s="21"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="21"/>
       <c r="J47" s="10"/>
       <c r="K47" s="11"/>
       <c r="L47" s="11"/>
@@ -3459,17 +3475,17 @@
       <c r="N47" s="12"/>
     </row>
     <row r="48" ht="13.5" customHeight="1">
-      <c r="A48" t="s" s="20">
-        <v>56</v>
-      </c>
-      <c r="B48" s="21"/>
-      <c r="C48" s="21"/>
-      <c r="D48" s="21"/>
-      <c r="E48" s="21"/>
-      <c r="F48" s="21"/>
-      <c r="G48" s="21"/>
-      <c r="H48" s="21"/>
-      <c r="I48" s="21"/>
+      <c r="A48" t="s" s="15">
+        <v>63</v>
+      </c>
+      <c r="B48" s="19"/>
+      <c r="C48" s="19"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="19"/>
+      <c r="F48" s="19"/>
+      <c r="G48" s="19"/>
+      <c r="H48" s="19"/>
+      <c r="I48" s="19"/>
       <c r="J48" s="10"/>
       <c r="K48" s="11"/>
       <c r="L48" s="11"/>
@@ -3477,15 +3493,15 @@
       <c r="N48" s="12"/>
     </row>
     <row r="49" ht="13.5" customHeight="1">
-      <c r="A49" s="17"/>
-      <c r="B49" s="17"/>
-      <c r="C49" s="17"/>
-      <c r="D49" s="18"/>
-      <c r="E49" s="18"/>
-      <c r="F49" s="18"/>
-      <c r="G49" s="18"/>
-      <c r="H49" s="18"/>
-      <c r="I49" s="18"/>
+      <c r="A49" s="16"/>
+      <c r="B49" s="16"/>
+      <c r="C49" s="16"/>
+      <c r="D49" s="17"/>
+      <c r="E49" s="17"/>
+      <c r="F49" s="17"/>
+      <c r="G49" s="17"/>
+      <c r="H49" s="17"/>
+      <c r="I49" s="17"/>
       <c r="J49" s="10"/>
       <c r="K49" s="11"/>
       <c r="L49" s="11"/>
@@ -3493,21 +3509,21 @@
       <c r="N49" s="12"/>
     </row>
     <row r="50" ht="13.5" customHeight="1">
-      <c r="A50" t="s" s="20">
-        <v>37</v>
-      </c>
-      <c r="B50" t="s" s="20">
-        <v>83</v>
-      </c>
-      <c r="C50" t="s" s="20">
-        <v>84</v>
-      </c>
-      <c r="D50" s="21"/>
-      <c r="E50" s="21"/>
-      <c r="F50" s="21"/>
-      <c r="G50" s="21"/>
-      <c r="H50" s="21"/>
-      <c r="I50" s="21"/>
+      <c r="A50" t="s" s="15">
+        <v>44</v>
+      </c>
+      <c r="B50" t="s" s="15">
+        <v>90</v>
+      </c>
+      <c r="C50" t="s" s="15">
+        <v>91</v>
+      </c>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="19"/>
+      <c r="H50" s="19"/>
+      <c r="I50" s="19"/>
       <c r="J50" s="10"/>
       <c r="K50" s="11"/>
       <c r="L50" s="11"/>
@@ -3515,21 +3531,21 @@
       <c r="N50" s="12"/>
     </row>
     <row r="51" ht="13.5" customHeight="1">
-      <c r="A51" t="s" s="22">
+      <c r="A51" t="s" s="20">
         <v>20</v>
       </c>
-      <c r="B51" t="s" s="22">
-        <v>53</v>
-      </c>
-      <c r="C51" t="s" s="22">
-        <v>54</v>
-      </c>
-      <c r="D51" s="23"/>
-      <c r="E51" s="23"/>
-      <c r="F51" s="23"/>
-      <c r="G51" s="23"/>
-      <c r="H51" s="23"/>
-      <c r="I51" s="23"/>
+      <c r="B51" t="s" s="20">
+        <v>60</v>
+      </c>
+      <c r="C51" t="s" s="20">
+        <v>61</v>
+      </c>
+      <c r="D51" s="21"/>
+      <c r="E51" s="21"/>
+      <c r="F51" s="21"/>
+      <c r="G51" s="21"/>
+      <c r="H51" s="21"/>
+      <c r="I51" s="21"/>
       <c r="J51" s="10"/>
       <c r="K51" s="11"/>
       <c r="L51" s="11"/>
@@ -3537,17 +3553,17 @@
       <c r="N51" s="12"/>
     </row>
     <row r="52" ht="13.5" customHeight="1">
-      <c r="A52" t="s" s="20">
-        <v>56</v>
-      </c>
-      <c r="B52" s="21"/>
-      <c r="C52" s="21"/>
-      <c r="D52" s="21"/>
-      <c r="E52" s="21"/>
-      <c r="F52" s="21"/>
-      <c r="G52" s="21"/>
-      <c r="H52" s="21"/>
-      <c r="I52" s="21"/>
+      <c r="A52" t="s" s="15">
+        <v>63</v>
+      </c>
+      <c r="B52" s="19"/>
+      <c r="C52" s="19"/>
+      <c r="D52" s="19"/>
+      <c r="E52" s="19"/>
+      <c r="F52" s="19"/>
+      <c r="G52" s="19"/>
+      <c r="H52" s="19"/>
+      <c r="I52" s="19"/>
       <c r="J52" s="10"/>
       <c r="K52" s="11"/>
       <c r="L52" s="11"/>
@@ -3555,15 +3571,15 @@
       <c r="N52" s="12"/>
     </row>
     <row r="53" ht="18" customHeight="1">
-      <c r="A53" s="24"/>
-      <c r="B53" s="25"/>
-      <c r="C53" s="25"/>
-      <c r="D53" s="25"/>
-      <c r="E53" s="25"/>
-      <c r="F53" s="25"/>
-      <c r="G53" s="25"/>
-      <c r="H53" s="25"/>
-      <c r="I53" s="25"/>
+      <c r="A53" s="22"/>
+      <c r="B53" s="23"/>
+      <c r="C53" s="23"/>
+      <c r="D53" s="23"/>
+      <c r="E53" s="23"/>
+      <c r="F53" s="23"/>
+      <c r="G53" s="23"/>
+      <c r="H53" s="23"/>
+      <c r="I53" s="23"/>
       <c r="J53" s="11"/>
       <c r="K53" s="11"/>
       <c r="L53" s="11"/>
@@ -3571,7 +3587,7 @@
       <c r="N53" s="12"/>
     </row>
     <row r="54" ht="18" customHeight="1">
-      <c r="A54" s="26"/>
+      <c r="A54" s="24"/>
       <c r="B54" s="11"/>
       <c r="C54" s="11"/>
       <c r="D54" s="11"/>
@@ -3587,7 +3603,7 @@
       <c r="N54" s="12"/>
     </row>
     <row r="55" ht="18" customHeight="1">
-      <c r="A55" s="26"/>
+      <c r="A55" s="24"/>
       <c r="B55" s="11"/>
       <c r="C55" s="11"/>
       <c r="D55" s="11"/>
@@ -3603,7 +3619,7 @@
       <c r="N55" s="12"/>
     </row>
     <row r="56" ht="18" customHeight="1">
-      <c r="A56" s="26"/>
+      <c r="A56" s="24"/>
       <c r="B56" s="11"/>
       <c r="C56" s="11"/>
       <c r="D56" s="11"/>
@@ -3619,7 +3635,7 @@
       <c r="N56" s="12"/>
     </row>
     <row r="57" ht="18" customHeight="1">
-      <c r="A57" s="26"/>
+      <c r="A57" s="24"/>
       <c r="B57" s="11"/>
       <c r="C57" s="11"/>
       <c r="D57" s="11"/>
@@ -3635,7 +3651,7 @@
       <c r="N57" s="12"/>
     </row>
     <row r="58" ht="18" customHeight="1">
-      <c r="A58" s="26"/>
+      <c r="A58" s="24"/>
       <c r="B58" s="11"/>
       <c r="C58" s="11"/>
       <c r="D58" s="11"/>
@@ -3651,7 +3667,7 @@
       <c r="N58" s="12"/>
     </row>
     <row r="59" ht="18" customHeight="1">
-      <c r="A59" s="26"/>
+      <c r="A59" s="24"/>
       <c r="B59" s="11"/>
       <c r="C59" s="11"/>
       <c r="D59" s="11"/>
@@ -3667,7 +3683,7 @@
       <c r="N59" s="12"/>
     </row>
     <row r="60" ht="18" customHeight="1">
-      <c r="A60" s="26"/>
+      <c r="A60" s="24"/>
       <c r="B60" s="11"/>
       <c r="C60" s="11"/>
       <c r="D60" s="11"/>
@@ -3683,7 +3699,7 @@
       <c r="N60" s="12"/>
     </row>
     <row r="61" ht="18" customHeight="1">
-      <c r="A61" s="26"/>
+      <c r="A61" s="24"/>
       <c r="B61" s="11"/>
       <c r="C61" s="11"/>
       <c r="D61" s="11"/>
@@ -3699,20 +3715,20 @@
       <c r="N61" s="12"/>
     </row>
     <row r="62" ht="18" customHeight="1">
-      <c r="A62" s="27"/>
-      <c r="B62" s="28"/>
-      <c r="C62" s="28"/>
-      <c r="D62" s="28"/>
-      <c r="E62" s="28"/>
-      <c r="F62" s="28"/>
-      <c r="G62" s="28"/>
-      <c r="H62" s="28"/>
-      <c r="I62" s="28"/>
-      <c r="J62" s="28"/>
-      <c r="K62" s="28"/>
-      <c r="L62" s="28"/>
-      <c r="M62" s="28"/>
-      <c r="N62" s="29"/>
+      <c r="A62" s="25"/>
+      <c r="B62" s="26"/>
+      <c r="C62" s="26"/>
+      <c r="D62" s="26"/>
+      <c r="E62" s="26"/>
+      <c r="F62" s="26"/>
+      <c r="G62" s="26"/>
+      <c r="H62" s="26"/>
+      <c r="I62" s="26"/>
+      <c r="J62" s="26"/>
+      <c r="K62" s="26"/>
+      <c r="L62" s="26"/>
+      <c r="M62" s="26"/>
+      <c r="N62" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
@@ -3736,1115 +3752,1127 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.3333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="27.3516" style="30" customWidth="1"/>
-    <col min="2" max="2" width="25.5" style="30" customWidth="1"/>
-    <col min="3" max="3" width="16.3516" style="30" customWidth="1"/>
-    <col min="4" max="4" width="53.1719" style="30" customWidth="1"/>
-    <col min="5" max="5" width="16.3516" style="30" customWidth="1"/>
-    <col min="6" max="6" width="16.3516" style="30" customWidth="1"/>
-    <col min="7" max="7" width="16.3516" style="30" customWidth="1"/>
-    <col min="8" max="8" width="16.3516" style="30" customWidth="1"/>
-    <col min="9" max="9" width="16.3516" style="30" customWidth="1"/>
-    <col min="10" max="10" width="16.3516" style="30" customWidth="1"/>
-    <col min="11" max="11" width="16.3516" style="30" customWidth="1"/>
-    <col min="12" max="256" width="17.3516" style="30" customWidth="1"/>
+    <col min="1" max="1" width="27.3516" style="28" customWidth="1"/>
+    <col min="2" max="2" width="25.5" style="28" customWidth="1"/>
+    <col min="3" max="3" width="16.3516" style="28" customWidth="1"/>
+    <col min="4" max="4" width="53.1719" style="28" customWidth="1"/>
+    <col min="5" max="5" width="16.3516" style="28" customWidth="1"/>
+    <col min="6" max="6" width="16.3516" style="28" customWidth="1"/>
+    <col min="7" max="7" width="16.3516" style="28" customWidth="1"/>
+    <col min="8" max="8" width="16.3516" style="28" customWidth="1"/>
+    <col min="9" max="9" width="16.3516" style="28" customWidth="1"/>
+    <col min="10" max="10" width="16.3516" style="28" customWidth="1"/>
+    <col min="11" max="11" width="16.3516" style="28" customWidth="1"/>
+    <col min="12" max="256" width="17.3516" style="28" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1">
-      <c r="A1" t="s" s="31">
-        <v>85</v>
-      </c>
-      <c r="B1" t="s" s="32">
+      <c r="A1" t="s" s="29">
+        <v>92</v>
+      </c>
+      <c r="B1" t="s" s="30">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="31">
+      <c r="C1" t="s" s="29">
         <v>2</v>
       </c>
-      <c r="D1" s="33"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="34"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="32"/>
     </row>
     <row r="2" ht="17.25" customHeight="1">
-      <c r="A2" t="s" s="38">
-        <v>86</v>
-      </c>
-      <c r="B2" t="s" s="39">
-        <v>87</v>
-      </c>
-      <c r="C2" t="s" s="40">
-        <v>88</v>
-      </c>
-      <c r="D2" s="41"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="44"/>
+      <c r="A2" t="s" s="36">
+        <v>93</v>
+      </c>
+      <c r="B2" t="s" s="37">
+        <v>94</v>
+      </c>
+      <c r="C2" t="s" s="38">
+        <v>95</v>
+      </c>
+      <c r="D2" s="39"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="42"/>
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
       <c r="J2" s="11"/>
-      <c r="K2" s="42"/>
+      <c r="K2" s="40"/>
     </row>
     <row r="3" ht="17.25" customHeight="1">
-      <c r="A3" t="s" s="38">
-        <v>86</v>
-      </c>
-      <c r="B3" t="s" s="39">
-        <v>89</v>
-      </c>
-      <c r="C3" t="s" s="40">
-        <v>90</v>
-      </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="44"/>
+      <c r="A3" t="s" s="36">
+        <v>93</v>
+      </c>
+      <c r="B3" t="s" s="37">
+        <v>96</v>
+      </c>
+      <c r="C3" t="s" s="38">
+        <v>97</v>
+      </c>
+      <c r="D3" s="39"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="42"/>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
-      <c r="K3" s="42"/>
+      <c r="K3" s="40"/>
     </row>
     <row r="4" ht="17.25" customHeight="1">
-      <c r="A4" t="s" s="38">
-        <v>86</v>
-      </c>
-      <c r="B4" t="s" s="39">
-        <v>91</v>
-      </c>
-      <c r="C4" t="s" s="40">
-        <v>92</v>
-      </c>
-      <c r="D4" s="41"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="44"/>
+      <c r="A4" t="s" s="36">
+        <v>93</v>
+      </c>
+      <c r="B4" t="s" s="37">
+        <v>98</v>
+      </c>
+      <c r="C4" t="s" s="38">
+        <v>99</v>
+      </c>
+      <c r="D4" s="39"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="42"/>
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
-      <c r="K4" s="42"/>
+      <c r="K4" s="40"/>
     </row>
     <row r="5" ht="17.25" customHeight="1">
-      <c r="A5" s="45"/>
-      <c r="B5" s="46"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="44"/>
+      <c r="A5" s="43"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="42"/>
       <c r="H5" s="11"/>
       <c r="I5" s="11"/>
       <c r="J5" s="11"/>
-      <c r="K5" s="42"/>
+      <c r="K5" s="40"/>
     </row>
     <row r="6" ht="17.25" customHeight="1">
-      <c r="A6" t="s" s="38">
-        <v>93</v>
-      </c>
-      <c r="B6" t="s" s="39">
+      <c r="A6" t="s" s="36">
+        <v>100</v>
+      </c>
+      <c r="B6" t="s" s="37">
         <v>19</v>
       </c>
-      <c r="C6" t="s" s="40">
-        <v>94</v>
-      </c>
-      <c r="D6" s="41"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="44"/>
+      <c r="C6" t="s" s="38">
+        <v>101</v>
+      </c>
+      <c r="D6" s="39"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="42"/>
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
-      <c r="K6" s="42"/>
+      <c r="K6" s="40"/>
     </row>
     <row r="7" ht="17.25" customHeight="1">
-      <c r="A7" t="s" s="38">
-        <v>93</v>
-      </c>
-      <c r="B7" t="s" s="39">
-        <v>70</v>
-      </c>
-      <c r="C7" t="s" s="40">
-        <v>95</v>
-      </c>
-      <c r="D7" s="41"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="44"/>
+      <c r="A7" t="s" s="36">
+        <v>100</v>
+      </c>
+      <c r="B7" t="s" s="37">
+        <v>77</v>
+      </c>
+      <c r="C7" t="s" s="38">
+        <v>102</v>
+      </c>
+      <c r="D7" s="39"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="42"/>
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
       <c r="J7" s="11"/>
-      <c r="K7" s="42"/>
+      <c r="K7" s="40"/>
     </row>
     <row r="8" ht="17.25" customHeight="1">
-      <c r="A8" s="38"/>
-      <c r="B8" s="46"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="44"/>
+      <c r="A8" s="36"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="42"/>
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
       <c r="J8" s="11"/>
-      <c r="K8" s="42"/>
+      <c r="K8" s="40"/>
     </row>
     <row r="9" ht="17.25" customHeight="1">
-      <c r="A9" t="s" s="38">
-        <v>96</v>
-      </c>
-      <c r="B9" t="s" s="39">
-        <v>97</v>
-      </c>
-      <c r="C9" t="s" s="40">
-        <v>98</v>
-      </c>
-      <c r="D9" s="41"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="44"/>
+      <c r="A9" t="s" s="36">
+        <v>103</v>
+      </c>
+      <c r="B9" t="s" s="37">
+        <v>104</v>
+      </c>
+      <c r="C9" t="s" s="38">
+        <v>105</v>
+      </c>
+      <c r="D9" s="39"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="42"/>
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
       <c r="J9" s="11"/>
-      <c r="K9" s="42"/>
+      <c r="K9" s="40"/>
     </row>
     <row r="10" ht="32.25" customHeight="1">
-      <c r="A10" t="s" s="38">
-        <v>96</v>
-      </c>
-      <c r="B10" t="s" s="39">
-        <v>99</v>
-      </c>
-      <c r="C10" t="s" s="40">
-        <v>100</v>
-      </c>
-      <c r="D10" s="41"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="44"/>
+      <c r="A10" t="s" s="36">
+        <v>103</v>
+      </c>
+      <c r="B10" t="s" s="37">
+        <v>106</v>
+      </c>
+      <c r="C10" t="s" s="38">
+        <v>107</v>
+      </c>
+      <c r="D10" s="39"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="42"/>
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
-      <c r="K10" s="42"/>
+      <c r="K10" s="40"/>
     </row>
     <row r="11" ht="17.25" customHeight="1">
-      <c r="A11" t="s" s="38">
-        <v>96</v>
-      </c>
-      <c r="B11" t="s" s="39">
-        <v>101</v>
-      </c>
-      <c r="C11" t="s" s="40">
-        <v>102</v>
-      </c>
-      <c r="D11" s="41"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="44"/>
+      <c r="A11" t="s" s="36">
+        <v>103</v>
+      </c>
+      <c r="B11" t="s" s="37">
+        <v>108</v>
+      </c>
+      <c r="C11" t="s" s="38">
+        <v>109</v>
+      </c>
+      <c r="D11" s="39"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="42"/>
       <c r="H11" s="11"/>
       <c r="I11" s="11"/>
       <c r="J11" s="11"/>
-      <c r="K11" s="42"/>
+      <c r="K11" s="40"/>
     </row>
     <row r="12" ht="17.25" customHeight="1">
-      <c r="A12" t="s" s="38">
-        <v>96</v>
-      </c>
-      <c r="B12" t="s" s="39">
+      <c r="A12" t="s" s="36">
         <v>103</v>
       </c>
-      <c r="C12" t="s" s="40">
-        <v>104</v>
-      </c>
-      <c r="D12" s="41"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="44"/>
+      <c r="B12" t="s" s="37">
+        <v>110</v>
+      </c>
+      <c r="C12" t="s" s="38">
+        <v>111</v>
+      </c>
+      <c r="D12" s="39"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="42"/>
       <c r="H12" s="11"/>
       <c r="I12" s="11"/>
       <c r="J12" s="11"/>
-      <c r="K12" s="42"/>
+      <c r="K12" s="40"/>
     </row>
     <row r="13" ht="17.25" customHeight="1">
-      <c r="A13" t="s" s="38">
-        <v>96</v>
-      </c>
-      <c r="B13" t="s" s="39">
-        <v>105</v>
-      </c>
-      <c r="C13" t="s" s="40">
-        <v>106</v>
-      </c>
-      <c r="D13" s="41"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="44"/>
+      <c r="A13" t="s" s="36">
+        <v>103</v>
+      </c>
+      <c r="B13" t="s" s="37">
+        <v>112</v>
+      </c>
+      <c r="C13" t="s" s="38">
+        <v>113</v>
+      </c>
+      <c r="D13" s="39"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="42"/>
       <c r="H13" s="11"/>
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
-      <c r="K13" s="42"/>
+      <c r="K13" s="40"/>
     </row>
     <row r="14" ht="17.25" customHeight="1">
-      <c r="A14" t="s" s="38">
-        <v>96</v>
-      </c>
-      <c r="B14" t="s" s="39">
-        <v>107</v>
-      </c>
-      <c r="C14" t="s" s="40">
-        <v>108</v>
-      </c>
-      <c r="D14" s="41"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="44"/>
+      <c r="A14" t="s" s="36">
+        <v>103</v>
+      </c>
+      <c r="B14" t="s" s="37">
+        <v>114</v>
+      </c>
+      <c r="C14" t="s" s="38">
+        <v>115</v>
+      </c>
+      <c r="D14" s="39"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="42"/>
       <c r="H14" s="11"/>
       <c r="I14" s="11"/>
       <c r="J14" s="11"/>
-      <c r="K14" s="42"/>
+      <c r="K14" s="40"/>
     </row>
     <row r="15" ht="32.25" customHeight="1">
-      <c r="A15" t="s" s="38">
-        <v>96</v>
-      </c>
-      <c r="B15" t="s" s="39">
-        <v>109</v>
-      </c>
-      <c r="C15" t="s" s="40">
-        <v>110</v>
-      </c>
-      <c r="D15" s="41"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="44"/>
+      <c r="A15" t="s" s="36">
+        <v>103</v>
+      </c>
+      <c r="B15" t="s" s="37">
+        <v>116</v>
+      </c>
+      <c r="C15" t="s" s="38">
+        <v>117</v>
+      </c>
+      <c r="D15" s="39"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="42"/>
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
       <c r="J15" s="11"/>
-      <c r="K15" s="42"/>
+      <c r="K15" s="40"/>
     </row>
     <row r="16" ht="17.25" customHeight="1">
-      <c r="A16" t="s" s="38">
-        <v>96</v>
-      </c>
-      <c r="B16" t="s" s="39">
-        <v>111</v>
-      </c>
-      <c r="C16" t="s" s="40">
-        <v>112</v>
-      </c>
-      <c r="D16" s="41"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="44"/>
+      <c r="A16" t="s" s="36">
+        <v>103</v>
+      </c>
+      <c r="B16" t="s" s="37">
+        <v>118</v>
+      </c>
+      <c r="C16" t="s" s="38">
+        <v>119</v>
+      </c>
+      <c r="D16" s="39"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="42"/>
       <c r="H16" s="11"/>
       <c r="I16" s="11"/>
       <c r="J16" s="11"/>
-      <c r="K16" s="42"/>
+      <c r="K16" s="40"/>
     </row>
     <row r="17" ht="17.25" customHeight="1">
-      <c r="A17" s="48"/>
-      <c r="B17" s="46"/>
-      <c r="C17" s="47"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="44"/>
+      <c r="A17" s="46"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="42"/>
       <c r="H17" s="11"/>
       <c r="I17" s="11"/>
       <c r="J17" s="11"/>
-      <c r="K17" s="42"/>
+      <c r="K17" s="40"/>
     </row>
     <row r="18" ht="32.25" customHeight="1">
-      <c r="A18" t="s" s="38">
-        <v>35</v>
-      </c>
-      <c r="B18" t="s" s="39">
-        <v>113</v>
-      </c>
-      <c r="C18" t="s" s="40">
-        <v>114</v>
-      </c>
-      <c r="D18" s="49"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="44"/>
+      <c r="A18" t="s" s="36">
+        <v>42</v>
+      </c>
+      <c r="B18" t="s" s="37">
+        <v>120</v>
+      </c>
+      <c r="C18" t="s" s="38">
+        <v>121</v>
+      </c>
+      <c r="D18" s="47"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="42"/>
       <c r="H18" s="11"/>
       <c r="I18" s="11"/>
       <c r="J18" s="11"/>
-      <c r="K18" s="42"/>
+      <c r="K18" s="40"/>
     </row>
     <row r="19" ht="32.25" customHeight="1">
-      <c r="A19" t="s" s="38">
-        <v>35</v>
-      </c>
-      <c r="B19" t="s" s="39">
-        <v>115</v>
-      </c>
-      <c r="C19" t="s" s="40">
-        <v>116</v>
-      </c>
-      <c r="D19" s="50"/>
-      <c r="E19" s="51"/>
-      <c r="F19" s="52"/>
-      <c r="G19" s="44"/>
+      <c r="A19" t="s" s="36">
+        <v>42</v>
+      </c>
+      <c r="B19" t="s" s="37">
+        <v>122</v>
+      </c>
+      <c r="C19" t="s" s="38">
+        <v>123</v>
+      </c>
+      <c r="D19" s="48"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="42"/>
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
       <c r="J19" s="11"/>
-      <c r="K19" s="42"/>
+      <c r="K19" s="40"/>
     </row>
     <row r="20" ht="17.25" customHeight="1">
-      <c r="A20" t="s" s="38">
-        <v>35</v>
-      </c>
-      <c r="B20" t="s" s="39">
-        <v>91</v>
-      </c>
-      <c r="C20" t="s" s="40">
-        <v>117</v>
-      </c>
-      <c r="D20" s="50"/>
-      <c r="E20" s="51"/>
-      <c r="F20" s="52"/>
-      <c r="G20" s="44"/>
+      <c r="A20" t="s" s="36">
+        <v>42</v>
+      </c>
+      <c r="B20" t="s" s="37">
+        <v>98</v>
+      </c>
+      <c r="C20" t="s" s="38">
+        <v>124</v>
+      </c>
+      <c r="D20" s="48"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="50"/>
+      <c r="G20" s="42"/>
       <c r="H20" s="11"/>
       <c r="I20" s="11"/>
       <c r="J20" s="11"/>
-      <c r="K20" s="42"/>
+      <c r="K20" s="40"/>
     </row>
     <row r="21" ht="17.25" customHeight="1">
-      <c r="A21" t="s" s="38">
-        <v>35</v>
-      </c>
-      <c r="B21" t="s" s="39">
-        <v>118</v>
-      </c>
-      <c r="C21" t="s" s="40">
-        <v>119</v>
-      </c>
-      <c r="D21" s="50"/>
-      <c r="E21" s="51"/>
-      <c r="F21" s="52"/>
-      <c r="G21" s="44"/>
+      <c r="A21" t="s" s="36">
+        <v>42</v>
+      </c>
+      <c r="B21" t="s" s="37">
+        <v>125</v>
+      </c>
+      <c r="C21" t="s" s="38">
+        <v>126</v>
+      </c>
+      <c r="D21" s="48"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="50"/>
+      <c r="G21" s="42"/>
       <c r="H21" s="11"/>
       <c r="I21" s="11"/>
       <c r="J21" s="11"/>
-      <c r="K21" s="42"/>
+      <c r="K21" s="40"/>
     </row>
     <row r="22" ht="32.25" customHeight="1">
-      <c r="A22" t="s" s="38">
-        <v>35</v>
-      </c>
-      <c r="B22" t="s" s="39">
-        <v>120</v>
-      </c>
-      <c r="C22" t="s" s="40">
-        <v>121</v>
-      </c>
-      <c r="D22" s="50"/>
-      <c r="E22" s="51"/>
-      <c r="F22" s="52"/>
-      <c r="G22" s="44"/>
+      <c r="A22" t="s" s="36">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s" s="37">
+        <v>127</v>
+      </c>
+      <c r="C22" t="s" s="38">
+        <v>128</v>
+      </c>
+      <c r="D22" s="48"/>
+      <c r="E22" s="49"/>
+      <c r="F22" s="50"/>
+      <c r="G22" s="42"/>
       <c r="H22" s="11"/>
       <c r="I22" s="11"/>
       <c r="J22" s="11"/>
-      <c r="K22" s="42"/>
+      <c r="K22" s="40"/>
     </row>
     <row r="23" ht="17.25" customHeight="1">
-      <c r="A23" t="s" s="38">
-        <v>35</v>
-      </c>
-      <c r="B23" t="s" s="39">
-        <v>122</v>
-      </c>
-      <c r="C23" t="s" s="40">
-        <v>123</v>
-      </c>
-      <c r="D23" s="50"/>
-      <c r="E23" s="51"/>
-      <c r="F23" s="52"/>
-      <c r="G23" s="44"/>
+      <c r="A23" t="s" s="36">
+        <v>42</v>
+      </c>
+      <c r="B23" t="s" s="37">
+        <v>129</v>
+      </c>
+      <c r="C23" t="s" s="38">
+        <v>130</v>
+      </c>
+      <c r="D23" s="48"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="42"/>
       <c r="H23" s="11"/>
       <c r="I23" s="11"/>
       <c r="J23" s="11"/>
-      <c r="K23" s="42"/>
+      <c r="K23" s="40"/>
     </row>
     <row r="24" ht="17.25" customHeight="1">
-      <c r="A24" t="s" s="38">
-        <v>35</v>
-      </c>
-      <c r="B24" t="s" s="39">
-        <v>124</v>
-      </c>
-      <c r="C24" t="s" s="40">
-        <v>125</v>
-      </c>
-      <c r="D24" s="50"/>
-      <c r="E24" s="51"/>
-      <c r="F24" s="52"/>
-      <c r="G24" s="44"/>
+      <c r="A24" t="s" s="36">
+        <v>42</v>
+      </c>
+      <c r="B24" t="s" s="37">
+        <v>131</v>
+      </c>
+      <c r="C24" t="s" s="38">
+        <v>132</v>
+      </c>
+      <c r="D24" s="48"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="50"/>
+      <c r="G24" s="42"/>
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
       <c r="J24" s="11"/>
-      <c r="K24" s="42"/>
+      <c r="K24" s="40"/>
     </row>
     <row r="25" ht="32.25" customHeight="1">
-      <c r="A25" t="s" s="38">
-        <v>35</v>
-      </c>
-      <c r="B25" t="s" s="39">
-        <v>87</v>
-      </c>
-      <c r="C25" t="s" s="40">
-        <v>126</v>
-      </c>
-      <c r="D25" s="50"/>
-      <c r="E25" s="51"/>
-      <c r="F25" s="52"/>
-      <c r="G25" s="44"/>
+      <c r="A25" t="s" s="36">
+        <v>42</v>
+      </c>
+      <c r="B25" t="s" s="37">
+        <v>94</v>
+      </c>
+      <c r="C25" t="s" s="38">
+        <v>133</v>
+      </c>
+      <c r="D25" s="48"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="50"/>
+      <c r="G25" s="42"/>
       <c r="H25" s="11"/>
       <c r="I25" s="11"/>
       <c r="J25" s="11"/>
-      <c r="K25" s="42"/>
+      <c r="K25" s="40"/>
     </row>
     <row r="26" ht="17.25" customHeight="1">
-      <c r="A26" t="s" s="38">
-        <v>35</v>
-      </c>
-      <c r="B26" t="s" s="39">
-        <v>127</v>
-      </c>
-      <c r="C26" t="s" s="40">
-        <v>128</v>
-      </c>
-      <c r="D26" s="50"/>
-      <c r="E26" s="51"/>
-      <c r="F26" s="52"/>
-      <c r="G26" s="44"/>
+      <c r="A26" t="s" s="36">
+        <v>42</v>
+      </c>
+      <c r="B26" t="s" s="37">
+        <v>134</v>
+      </c>
+      <c r="C26" t="s" s="38">
+        <v>135</v>
+      </c>
+      <c r="D26" s="48"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="50"/>
+      <c r="G26" s="42"/>
       <c r="H26" s="11"/>
       <c r="I26" s="11"/>
       <c r="J26" s="11"/>
-      <c r="K26" s="42"/>
+      <c r="K26" s="40"/>
     </row>
     <row r="27" ht="17.25" customHeight="1">
-      <c r="A27" t="s" s="38">
-        <v>35</v>
-      </c>
-      <c r="B27" t="s" s="39">
-        <v>89</v>
-      </c>
-      <c r="C27" t="s" s="40">
-        <v>129</v>
-      </c>
-      <c r="D27" s="50"/>
-      <c r="E27" s="51"/>
-      <c r="F27" s="52"/>
-      <c r="G27" s="44"/>
+      <c r="A27" t="s" s="36">
+        <v>42</v>
+      </c>
+      <c r="B27" t="s" s="37">
+        <v>96</v>
+      </c>
+      <c r="C27" t="s" s="38">
+        <v>136</v>
+      </c>
+      <c r="D27" s="48"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="50"/>
+      <c r="G27" s="42"/>
       <c r="H27" s="11"/>
       <c r="I27" s="11"/>
       <c r="J27" s="11"/>
-      <c r="K27" s="42"/>
+      <c r="K27" s="40"/>
     </row>
     <row r="28" ht="17.25" customHeight="1">
-      <c r="A28" t="s" s="38">
-        <v>35</v>
-      </c>
-      <c r="B28" t="s" s="39">
-        <v>130</v>
-      </c>
-      <c r="C28" t="s" s="40">
-        <v>131</v>
-      </c>
-      <c r="D28" s="50"/>
-      <c r="E28" s="51"/>
-      <c r="F28" s="52"/>
-      <c r="G28" s="44"/>
+      <c r="A28" t="s" s="36">
+        <v>42</v>
+      </c>
+      <c r="B28" t="s" s="37">
+        <v>137</v>
+      </c>
+      <c r="C28" t="s" s="38">
+        <v>138</v>
+      </c>
+      <c r="D28" s="48"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="42"/>
       <c r="H28" s="11"/>
       <c r="I28" s="11"/>
       <c r="J28" s="11"/>
-      <c r="K28" s="42"/>
+      <c r="K28" s="40"/>
     </row>
     <row r="29" ht="17.25" customHeight="1">
-      <c r="A29" t="s" s="38">
-        <v>35</v>
-      </c>
-      <c r="B29" t="s" s="39">
-        <v>132</v>
-      </c>
-      <c r="C29" t="s" s="40">
-        <v>133</v>
-      </c>
-      <c r="D29" s="50"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="52"/>
-      <c r="G29" s="44"/>
+      <c r="A29" t="s" s="36">
+        <v>42</v>
+      </c>
+      <c r="B29" t="s" s="37">
+        <v>139</v>
+      </c>
+      <c r="C29" t="s" s="38">
+        <v>140</v>
+      </c>
+      <c r="D29" s="48"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="50"/>
+      <c r="G29" s="42"/>
       <c r="H29" s="11"/>
       <c r="I29" s="11"/>
       <c r="J29" s="11"/>
-      <c r="K29" s="42"/>
+      <c r="K29" s="40"/>
     </row>
     <row r="30" ht="17.25" customHeight="1">
-      <c r="A30" t="s" s="38">
-        <v>35</v>
-      </c>
-      <c r="B30" t="s" s="39">
-        <v>134</v>
-      </c>
-      <c r="C30" t="s" s="40">
-        <v>135</v>
-      </c>
-      <c r="D30" s="50"/>
-      <c r="E30" s="51"/>
-      <c r="F30" s="52"/>
-      <c r="G30" s="44"/>
+      <c r="A30" t="s" s="36">
+        <v>42</v>
+      </c>
+      <c r="B30" t="s" s="37">
+        <v>141</v>
+      </c>
+      <c r="C30" t="s" s="38">
+        <v>142</v>
+      </c>
+      <c r="D30" s="48"/>
+      <c r="E30" s="49"/>
+      <c r="F30" s="50"/>
+      <c r="G30" s="42"/>
       <c r="H30" s="11"/>
       <c r="I30" s="11"/>
       <c r="J30" s="11"/>
-      <c r="K30" s="42"/>
+      <c r="K30" s="40"/>
     </row>
     <row r="31" ht="17.25" customHeight="1">
-      <c r="A31" t="s" s="38">
-        <v>35</v>
-      </c>
-      <c r="B31" t="s" s="39">
-        <v>136</v>
-      </c>
-      <c r="C31" t="s" s="40">
-        <v>137</v>
-      </c>
-      <c r="D31" s="50"/>
-      <c r="E31" s="51"/>
-      <c r="F31" s="52"/>
-      <c r="G31" s="44"/>
+      <c r="A31" t="s" s="36">
+        <v>42</v>
+      </c>
+      <c r="B31" t="s" s="37">
+        <v>143</v>
+      </c>
+      <c r="C31" t="s" s="38">
+        <v>144</v>
+      </c>
+      <c r="D31" s="48"/>
+      <c r="E31" s="49"/>
+      <c r="F31" s="50"/>
+      <c r="G31" s="42"/>
       <c r="H31" s="11"/>
       <c r="I31" s="11"/>
       <c r="J31" s="11"/>
-      <c r="K31" s="42"/>
+      <c r="K31" s="40"/>
     </row>
     <row r="32" ht="17.25" customHeight="1">
-      <c r="A32" t="s" s="38">
-        <v>35</v>
-      </c>
-      <c r="B32" t="s" s="39">
-        <v>138</v>
-      </c>
-      <c r="C32" t="s" s="40">
-        <v>139</v>
-      </c>
-      <c r="D32" s="50"/>
-      <c r="E32" s="51"/>
-      <c r="F32" s="52"/>
-      <c r="G32" s="44"/>
+      <c r="A32" t="s" s="36">
+        <v>42</v>
+      </c>
+      <c r="B32" t="s" s="37">
+        <v>145</v>
+      </c>
+      <c r="C32" t="s" s="38">
+        <v>146</v>
+      </c>
+      <c r="D32" s="48"/>
+      <c r="E32" s="49"/>
+      <c r="F32" s="50"/>
+      <c r="G32" s="42"/>
       <c r="H32" s="11"/>
       <c r="I32" s="11"/>
       <c r="J32" s="11"/>
-      <c r="K32" s="42"/>
+      <c r="K32" s="40"/>
     </row>
     <row r="33" ht="17.25" customHeight="1">
-      <c r="A33" t="s" s="38">
-        <v>35</v>
-      </c>
-      <c r="B33" t="s" s="39">
-        <v>140</v>
-      </c>
-      <c r="C33" t="s" s="40">
-        <v>141</v>
-      </c>
-      <c r="D33" s="50"/>
-      <c r="E33" s="51"/>
-      <c r="F33" s="52"/>
-      <c r="G33" s="44"/>
+      <c r="A33" t="s" s="36">
+        <v>42</v>
+      </c>
+      <c r="B33" t="s" s="37">
+        <v>147</v>
+      </c>
+      <c r="C33" t="s" s="38">
+        <v>148</v>
+      </c>
+      <c r="D33" s="48"/>
+      <c r="E33" s="49"/>
+      <c r="F33" s="50"/>
+      <c r="G33" s="42"/>
       <c r="H33" s="11"/>
       <c r="I33" s="11"/>
       <c r="J33" s="11"/>
-      <c r="K33" s="42"/>
+      <c r="K33" s="40"/>
     </row>
     <row r="34" ht="17.25" customHeight="1">
-      <c r="A34" t="s" s="38">
-        <v>35</v>
-      </c>
-      <c r="B34" t="s" s="39">
-        <v>142</v>
-      </c>
-      <c r="C34" t="s" s="40">
-        <v>143</v>
-      </c>
-      <c r="D34" s="50"/>
-      <c r="E34" s="51"/>
-      <c r="F34" s="52"/>
-      <c r="G34" s="44"/>
+      <c r="A34" t="s" s="36">
+        <v>42</v>
+      </c>
+      <c r="B34" t="s" s="37">
+        <v>149</v>
+      </c>
+      <c r="C34" t="s" s="38">
+        <v>150</v>
+      </c>
+      <c r="D34" s="48"/>
+      <c r="E34" s="49"/>
+      <c r="F34" s="50"/>
+      <c r="G34" s="42"/>
       <c r="H34" s="11"/>
       <c r="I34" s="11"/>
       <c r="J34" s="11"/>
-      <c r="K34" s="42"/>
+      <c r="K34" s="40"/>
     </row>
     <row r="35" ht="17.25" customHeight="1">
-      <c r="A35" t="s" s="38">
-        <v>35</v>
-      </c>
-      <c r="B35" t="s" s="39">
-        <v>144</v>
-      </c>
-      <c r="C35" t="s" s="40">
-        <v>145</v>
-      </c>
-      <c r="D35" s="50"/>
-      <c r="E35" s="51"/>
-      <c r="F35" s="52"/>
-      <c r="G35" s="44"/>
+      <c r="A35" t="s" s="36">
+        <v>42</v>
+      </c>
+      <c r="B35" t="s" s="37">
+        <v>151</v>
+      </c>
+      <c r="C35" t="s" s="38">
+        <v>152</v>
+      </c>
+      <c r="D35" s="48"/>
+      <c r="E35" s="49"/>
+      <c r="F35" s="50"/>
+      <c r="G35" s="42"/>
       <c r="H35" s="11"/>
       <c r="I35" s="11"/>
       <c r="J35" s="11"/>
-      <c r="K35" s="42"/>
+      <c r="K35" s="40"/>
     </row>
     <row r="36" ht="17.25" customHeight="1">
-      <c r="A36" t="s" s="38">
-        <v>35</v>
-      </c>
-      <c r="B36" t="s" s="39">
-        <v>146</v>
-      </c>
-      <c r="C36" t="s" s="40">
-        <v>147</v>
-      </c>
-      <c r="D36" s="50"/>
-      <c r="E36" s="51"/>
-      <c r="F36" s="52"/>
-      <c r="G36" s="44"/>
+      <c r="A36" t="s" s="36">
+        <v>42</v>
+      </c>
+      <c r="B36" t="s" s="37">
+        <v>153</v>
+      </c>
+      <c r="C36" t="s" s="38">
+        <v>154</v>
+      </c>
+      <c r="D36" s="48"/>
+      <c r="E36" s="49"/>
+      <c r="F36" s="50"/>
+      <c r="G36" s="42"/>
       <c r="H36" s="11"/>
       <c r="I36" s="11"/>
       <c r="J36" s="11"/>
-      <c r="K36" s="42"/>
+      <c r="K36" s="40"/>
     </row>
     <row r="37" ht="17.25" customHeight="1">
-      <c r="A37" s="53"/>
-      <c r="B37" s="54"/>
-      <c r="C37" s="31"/>
-      <c r="D37" s="50"/>
-      <c r="E37" s="51"/>
-      <c r="F37" s="52"/>
-      <c r="G37" s="44"/>
+      <c r="A37" s="51"/>
+      <c r="B37" s="52"/>
+      <c r="C37" s="29"/>
+      <c r="D37" s="48"/>
+      <c r="E37" s="49"/>
+      <c r="F37" s="50"/>
+      <c r="G37" s="42"/>
       <c r="H37" s="11"/>
       <c r="I37" s="11"/>
       <c r="J37" s="11"/>
-      <c r="K37" s="42"/>
+      <c r="K37" s="40"/>
     </row>
     <row r="38" ht="17.25" customHeight="1">
-      <c r="A38" t="s" s="53">
-        <v>148</v>
-      </c>
-      <c r="B38" t="s" s="54">
-        <v>149</v>
-      </c>
-      <c r="C38" t="s" s="31">
-        <v>150</v>
-      </c>
-      <c r="D38" s="50"/>
-      <c r="E38" s="51"/>
-      <c r="F38" s="52"/>
-      <c r="G38" s="44"/>
+      <c r="A38" t="s" s="51">
+        <v>155</v>
+      </c>
+      <c r="B38" t="s" s="52">
+        <v>156</v>
+      </c>
+      <c r="C38" t="s" s="29">
+        <v>157</v>
+      </c>
+      <c r="D38" s="48"/>
+      <c r="E38" s="49"/>
+      <c r="F38" s="50"/>
+      <c r="G38" s="42"/>
       <c r="H38" s="11"/>
       <c r="I38" s="11"/>
       <c r="J38" s="11"/>
-      <c r="K38" s="42"/>
+      <c r="K38" s="40"/>
     </row>
     <row r="39" ht="17.25" customHeight="1">
-      <c r="A39" t="s" s="53">
-        <v>148</v>
-      </c>
-      <c r="B39" t="s" s="54">
-        <v>151</v>
-      </c>
-      <c r="C39" t="s" s="31">
-        <v>152</v>
-      </c>
-      <c r="D39" s="50"/>
-      <c r="E39" s="51"/>
-      <c r="F39" s="52"/>
-      <c r="G39" s="44"/>
+      <c r="A39" t="s" s="51">
+        <v>155</v>
+      </c>
+      <c r="B39" t="s" s="52">
+        <v>158</v>
+      </c>
+      <c r="C39" t="s" s="29">
+        <v>159</v>
+      </c>
+      <c r="D39" s="48"/>
+      <c r="E39" s="49"/>
+      <c r="F39" s="50"/>
+      <c r="G39" s="42"/>
       <c r="H39" s="11"/>
       <c r="I39" s="11"/>
       <c r="J39" s="11"/>
-      <c r="K39" s="42"/>
+      <c r="K39" s="40"/>
     </row>
     <row r="40" ht="17.25" customHeight="1">
-      <c r="A40" t="s" s="53">
-        <v>148</v>
-      </c>
-      <c r="B40" t="s" s="54">
-        <v>153</v>
-      </c>
-      <c r="C40" t="s" s="31">
-        <v>154</v>
-      </c>
-      <c r="D40" s="50"/>
-      <c r="E40" s="51"/>
-      <c r="F40" s="52"/>
-      <c r="G40" s="44"/>
+      <c r="A40" t="s" s="51">
+        <v>155</v>
+      </c>
+      <c r="B40" t="s" s="52">
+        <v>160</v>
+      </c>
+      <c r="C40" t="s" s="29">
+        <v>161</v>
+      </c>
+      <c r="D40" s="48"/>
+      <c r="E40" s="49"/>
+      <c r="F40" s="50"/>
+      <c r="G40" s="42"/>
       <c r="H40" s="11"/>
       <c r="I40" s="11"/>
       <c r="J40" s="11"/>
-      <c r="K40" s="42"/>
+      <c r="K40" s="40"/>
     </row>
     <row r="41" ht="17.25" customHeight="1">
-      <c r="A41" t="s" s="53">
-        <v>148</v>
-      </c>
-      <c r="B41" t="s" s="54">
+      <c r="A41" t="s" s="51">
         <v>155</v>
       </c>
-      <c r="C41" t="s" s="31">
-        <v>156</v>
-      </c>
-      <c r="D41" s="50"/>
-      <c r="E41" s="51"/>
-      <c r="F41" s="52"/>
-      <c r="G41" s="44"/>
+      <c r="B41" t="s" s="52">
+        <v>162</v>
+      </c>
+      <c r="C41" t="s" s="29">
+        <v>163</v>
+      </c>
+      <c r="D41" s="48"/>
+      <c r="E41" s="49"/>
+      <c r="F41" s="50"/>
+      <c r="G41" s="42"/>
       <c r="H41" s="11"/>
       <c r="I41" s="11"/>
       <c r="J41" s="11"/>
-      <c r="K41" s="42"/>
+      <c r="K41" s="40"/>
     </row>
     <row r="42" ht="17.25" customHeight="1">
-      <c r="A42" t="s" s="53">
-        <v>148</v>
-      </c>
-      <c r="B42" t="s" s="54">
-        <v>157</v>
-      </c>
-      <c r="C42" t="s" s="31">
-        <v>158</v>
-      </c>
-      <c r="D42" s="50"/>
-      <c r="E42" s="51"/>
-      <c r="F42" s="52"/>
-      <c r="G42" s="44"/>
+      <c r="A42" t="s" s="51">
+        <v>155</v>
+      </c>
+      <c r="B42" t="s" s="52">
+        <v>164</v>
+      </c>
+      <c r="C42" t="s" s="29">
+        <v>165</v>
+      </c>
+      <c r="D42" s="48"/>
+      <c r="E42" s="49"/>
+      <c r="F42" s="50"/>
+      <c r="G42" s="42"/>
       <c r="H42" s="11"/>
       <c r="I42" s="11"/>
       <c r="J42" s="11"/>
-      <c r="K42" s="42"/>
+      <c r="K42" s="40"/>
     </row>
     <row r="43" ht="17.25" customHeight="1">
-      <c r="A43" t="s" s="53">
-        <v>148</v>
-      </c>
-      <c r="B43" t="s" s="54">
-        <v>89</v>
-      </c>
-      <c r="C43" t="s" s="31">
-        <v>159</v>
-      </c>
-      <c r="D43" s="50"/>
-      <c r="E43" s="51"/>
-      <c r="F43" s="52"/>
-      <c r="G43" s="44"/>
+      <c r="A43" t="s" s="51">
+        <v>155</v>
+      </c>
+      <c r="B43" t="s" s="52">
+        <v>96</v>
+      </c>
+      <c r="C43" t="s" s="29">
+        <v>166</v>
+      </c>
+      <c r="D43" s="48"/>
+      <c r="E43" s="49"/>
+      <c r="F43" s="50"/>
+      <c r="G43" s="42"/>
       <c r="H43" s="11"/>
       <c r="I43" s="11"/>
       <c r="J43" s="11"/>
-      <c r="K43" s="42"/>
+      <c r="K43" s="40"/>
     </row>
     <row r="44" ht="17.25" customHeight="1">
-      <c r="A44" t="s" s="53">
-        <v>148</v>
-      </c>
-      <c r="B44" t="s" s="54">
-        <v>132</v>
-      </c>
-      <c r="C44" t="s" s="31">
-        <v>133</v>
-      </c>
-      <c r="D44" s="50"/>
-      <c r="E44" s="51"/>
-      <c r="F44" s="52"/>
-      <c r="G44" s="44"/>
+      <c r="A44" t="s" s="51">
+        <v>155</v>
+      </c>
+      <c r="B44" t="s" s="52">
+        <v>139</v>
+      </c>
+      <c r="C44" t="s" s="29">
+        <v>140</v>
+      </c>
+      <c r="D44" s="48"/>
+      <c r="E44" s="49"/>
+      <c r="F44" s="50"/>
+      <c r="G44" s="42"/>
       <c r="H44" s="11"/>
       <c r="I44" s="11"/>
       <c r="J44" s="11"/>
-      <c r="K44" s="42"/>
+      <c r="K44" s="40"/>
     </row>
     <row r="45" ht="17.25" customHeight="1">
-      <c r="A45" t="s" s="53">
-        <v>148</v>
-      </c>
-      <c r="B45" t="s" s="54">
-        <v>160</v>
-      </c>
-      <c r="C45" t="s" s="31">
-        <v>161</v>
-      </c>
-      <c r="D45" s="50"/>
-      <c r="E45" s="51"/>
-      <c r="F45" s="52"/>
-      <c r="G45" s="44"/>
+      <c r="A45" t="s" s="51">
+        <v>155</v>
+      </c>
+      <c r="B45" t="s" s="52">
+        <v>167</v>
+      </c>
+      <c r="C45" t="s" s="29">
+        <v>168</v>
+      </c>
+      <c r="D45" s="48"/>
+      <c r="E45" s="49"/>
+      <c r="F45" s="50"/>
+      <c r="G45" s="42"/>
       <c r="H45" s="11"/>
       <c r="I45" s="11"/>
       <c r="J45" s="11"/>
-      <c r="K45" s="42"/>
+      <c r="K45" s="40"/>
     </row>
     <row r="46" ht="17.25" customHeight="1">
-      <c r="A46" t="s" s="53">
-        <v>148</v>
-      </c>
-      <c r="B46" t="s" s="54">
-        <v>162</v>
-      </c>
-      <c r="C46" t="s" s="31">
-        <v>163</v>
-      </c>
-      <c r="D46" s="50"/>
-      <c r="E46" s="51"/>
-      <c r="F46" s="52"/>
-      <c r="G46" s="44"/>
+      <c r="A46" t="s" s="51">
+        <v>155</v>
+      </c>
+      <c r="B46" t="s" s="52">
+        <v>169</v>
+      </c>
+      <c r="C46" t="s" s="29">
+        <v>170</v>
+      </c>
+      <c r="D46" s="48"/>
+      <c r="E46" s="49"/>
+      <c r="F46" s="50"/>
+      <c r="G46" s="42"/>
       <c r="H46" s="11"/>
       <c r="I46" s="11"/>
       <c r="J46" s="11"/>
-      <c r="K46" s="42"/>
+      <c r="K46" s="40"/>
     </row>
     <row r="47" ht="17.25" customHeight="1">
-      <c r="A47" t="s" s="53">
-        <v>148</v>
-      </c>
-      <c r="B47" t="s" s="54">
-        <v>49</v>
-      </c>
-      <c r="C47" t="s" s="31">
-        <v>164</v>
-      </c>
-      <c r="D47" s="50"/>
-      <c r="E47" s="51"/>
-      <c r="F47" s="52"/>
-      <c r="G47" s="44"/>
+      <c r="A47" t="s" s="51">
+        <v>155</v>
+      </c>
+      <c r="B47" t="s" s="52">
+        <v>56</v>
+      </c>
+      <c r="C47" t="s" s="29">
+        <v>171</v>
+      </c>
+      <c r="D47" s="48"/>
+      <c r="E47" s="49"/>
+      <c r="F47" s="50"/>
+      <c r="G47" s="42"/>
       <c r="H47" s="11"/>
       <c r="I47" s="11"/>
       <c r="J47" s="11"/>
-      <c r="K47" s="42"/>
+      <c r="K47" s="40"/>
     </row>
     <row r="48" ht="17.25" customHeight="1">
-      <c r="A48" s="53"/>
-      <c r="B48" s="54"/>
-      <c r="C48" s="31"/>
-      <c r="D48" s="50"/>
-      <c r="E48" s="51"/>
-      <c r="F48" s="52"/>
-      <c r="G48" s="44"/>
+      <c r="A48" s="51"/>
+      <c r="B48" s="52"/>
+      <c r="C48" s="29"/>
+      <c r="D48" s="48"/>
+      <c r="E48" s="49"/>
+      <c r="F48" s="50"/>
+      <c r="G48" s="42"/>
       <c r="H48" s="11"/>
       <c r="I48" s="11"/>
       <c r="J48" s="11"/>
-      <c r="K48" s="42"/>
+      <c r="K48" s="40"/>
     </row>
     <row r="49" ht="17.25" customHeight="1">
-      <c r="A49" s="55"/>
-      <c r="B49" s="56"/>
-      <c r="C49" s="57"/>
-      <c r="D49" s="50"/>
-      <c r="E49" s="51"/>
-      <c r="F49" s="52"/>
-      <c r="G49" s="44"/>
+      <c r="A49" s="53"/>
+      <c r="B49" s="54"/>
+      <c r="C49" s="55"/>
+      <c r="D49" s="48"/>
+      <c r="E49" s="49"/>
+      <c r="F49" s="50"/>
+      <c r="G49" s="42"/>
       <c r="H49" s="11"/>
       <c r="I49" s="11"/>
       <c r="J49" s="11"/>
-      <c r="K49" s="42"/>
+      <c r="K49" s="40"/>
     </row>
     <row r="50" ht="17.25" customHeight="1">
-      <c r="A50" t="s" s="53">
-        <v>165</v>
-      </c>
-      <c r="B50" t="s" s="54">
-        <v>45</v>
-      </c>
-      <c r="C50" t="s" s="31">
-        <v>166</v>
-      </c>
-      <c r="D50" s="50"/>
-      <c r="E50" s="51"/>
-      <c r="F50" s="52"/>
-      <c r="G50" s="44"/>
+      <c r="A50" t="s" s="51">
+        <v>172</v>
+      </c>
+      <c r="B50" t="s" s="52">
+        <v>52</v>
+      </c>
+      <c r="C50" t="s" s="29">
+        <v>173</v>
+      </c>
+      <c r="D50" s="48"/>
+      <c r="E50" s="49"/>
+      <c r="F50" s="50"/>
+      <c r="G50" s="42"/>
       <c r="H50" s="11"/>
       <c r="I50" s="11"/>
       <c r="J50" s="11"/>
-      <c r="K50" s="42"/>
+      <c r="K50" s="40"/>
     </row>
     <row r="51" ht="17.25" customHeight="1">
-      <c r="A51" t="s" s="53">
-        <v>165</v>
-      </c>
-      <c r="B51" t="s" s="54">
+      <c r="A51" t="s" s="51">
+        <v>172</v>
+      </c>
+      <c r="B51" t="s" s="52">
         <v>20</v>
       </c>
-      <c r="C51" t="s" s="31">
-        <v>167</v>
-      </c>
-      <c r="D51" s="50"/>
-      <c r="E51" s="51"/>
-      <c r="F51" s="52"/>
-      <c r="G51" s="44"/>
+      <c r="C51" t="s" s="29">
+        <v>174</v>
+      </c>
+      <c r="D51" s="48"/>
+      <c r="E51" s="49"/>
+      <c r="F51" s="50"/>
+      <c r="G51" s="42"/>
       <c r="H51" s="11"/>
       <c r="I51" s="11"/>
       <c r="J51" s="11"/>
-      <c r="K51" s="42"/>
+      <c r="K51" s="40"/>
     </row>
     <row r="52" ht="17.25" customHeight="1">
-      <c r="A52" t="s" s="53">
-        <v>165</v>
-      </c>
-      <c r="B52" t="s" s="54">
-        <v>168</v>
-      </c>
-      <c r="C52" t="s" s="31">
-        <v>169</v>
-      </c>
-      <c r="D52" s="50"/>
-      <c r="E52" s="51"/>
-      <c r="F52" s="52"/>
-      <c r="G52" s="44"/>
+      <c r="A52" t="s" s="51">
+        <v>172</v>
+      </c>
+      <c r="B52" t="s" s="52">
+        <v>175</v>
+      </c>
+      <c r="C52" t="s" s="29">
+        <v>176</v>
+      </c>
+      <c r="D52" s="48"/>
+      <c r="E52" s="49"/>
+      <c r="F52" s="50"/>
+      <c r="G52" s="42"/>
       <c r="H52" s="11"/>
       <c r="I52" s="11"/>
       <c r="J52" s="11"/>
-      <c r="K52" s="42"/>
+      <c r="K52" s="40"/>
     </row>
     <row r="53" ht="32.25" customHeight="1">
-      <c r="A53" t="s" s="53">
-        <v>165</v>
-      </c>
-      <c r="B53" t="s" s="54">
-        <v>170</v>
-      </c>
-      <c r="C53" t="s" s="31">
-        <v>171</v>
-      </c>
-      <c r="D53" s="50"/>
-      <c r="E53" s="51"/>
-      <c r="F53" s="52"/>
-      <c r="G53" s="44"/>
+      <c r="A53" t="s" s="51">
+        <v>172</v>
+      </c>
+      <c r="B53" t="s" s="52">
+        <v>177</v>
+      </c>
+      <c r="C53" t="s" s="29">
+        <v>178</v>
+      </c>
+      <c r="D53" s="48"/>
+      <c r="E53" s="49"/>
+      <c r="F53" s="50"/>
+      <c r="G53" s="42"/>
       <c r="H53" s="11"/>
       <c r="I53" s="11"/>
       <c r="J53" s="11"/>
-      <c r="K53" s="42"/>
+      <c r="K53" s="40"/>
     </row>
     <row r="54" ht="32.25" customHeight="1">
-      <c r="A54" t="s" s="53">
-        <v>165</v>
-      </c>
-      <c r="B54" t="s" s="54">
+      <c r="A54" t="s" s="51">
         <v>172</v>
       </c>
-      <c r="C54" t="s" s="31">
-        <v>173</v>
-      </c>
-      <c r="D54" s="50"/>
-      <c r="E54" s="51"/>
-      <c r="F54" s="52"/>
-      <c r="G54" s="44"/>
+      <c r="B54" t="s" s="52">
+        <v>179</v>
+      </c>
+      <c r="C54" t="s" s="29">
+        <v>180</v>
+      </c>
+      <c r="D54" s="48"/>
+      <c r="E54" s="49"/>
+      <c r="F54" s="50"/>
+      <c r="G54" s="42"/>
       <c r="H54" s="11"/>
       <c r="I54" s="11"/>
       <c r="J54" s="11"/>
-      <c r="K54" s="42"/>
+      <c r="K54" s="40"/>
     </row>
     <row r="55" ht="17.25" customHeight="1">
-      <c r="A55" s="55"/>
-      <c r="B55" s="56"/>
-      <c r="C55" s="57"/>
-      <c r="D55" s="50"/>
-      <c r="E55" s="51"/>
-      <c r="F55" s="52"/>
-      <c r="G55" s="44"/>
+      <c r="A55" s="53"/>
+      <c r="B55" s="54"/>
+      <c r="C55" s="55"/>
+      <c r="D55" s="48"/>
+      <c r="E55" s="49"/>
+      <c r="F55" s="50"/>
+      <c r="G55" s="42"/>
       <c r="H55" s="11"/>
       <c r="I55" s="11"/>
       <c r="J55" s="11"/>
-      <c r="K55" s="42"/>
+      <c r="K55" s="40"/>
     </row>
     <row r="56" ht="17.25" customHeight="1">
-      <c r="A56" t="s" s="53">
-        <v>174</v>
-      </c>
-      <c r="B56" t="s" s="54">
-        <v>175</v>
-      </c>
-      <c r="C56" t="s" s="31">
-        <v>176</v>
-      </c>
-      <c r="D56" s="50"/>
-      <c r="E56" s="51"/>
-      <c r="F56" s="52"/>
-      <c r="G56" s="44"/>
+      <c r="A56" t="s" s="51">
+        <v>181</v>
+      </c>
+      <c r="B56" t="s" s="52">
+        <v>182</v>
+      </c>
+      <c r="C56" t="s" s="29">
+        <v>183</v>
+      </c>
+      <c r="D56" s="48"/>
+      <c r="E56" s="49"/>
+      <c r="F56" s="50"/>
+      <c r="G56" s="42"/>
       <c r="H56" s="11"/>
       <c r="I56" s="11"/>
       <c r="J56" s="11"/>
-      <c r="K56" s="42"/>
+      <c r="K56" s="40"/>
     </row>
     <row r="57" ht="17.25" customHeight="1">
-      <c r="A57" t="s" s="53">
-        <v>174</v>
-      </c>
-      <c r="B57" t="s" s="54">
-        <v>65</v>
-      </c>
-      <c r="C57" t="s" s="31">
-        <v>177</v>
-      </c>
-      <c r="D57" s="50"/>
-      <c r="E57" s="51"/>
-      <c r="F57" s="52"/>
-      <c r="G57" s="44"/>
+      <c r="A57" t="s" s="51">
+        <v>181</v>
+      </c>
+      <c r="B57" t="s" s="52">
+        <v>72</v>
+      </c>
+      <c r="C57" t="s" s="29">
+        <v>184</v>
+      </c>
+      <c r="D57" s="48"/>
+      <c r="E57" s="49"/>
+      <c r="F57" s="50"/>
+      <c r="G57" s="42"/>
       <c r="H57" s="11"/>
       <c r="I57" s="11"/>
       <c r="J57" s="11"/>
-      <c r="K57" s="42"/>
+      <c r="K57" s="40"/>
     </row>
     <row r="58" ht="17.25" customHeight="1">
-      <c r="A58" s="55"/>
-      <c r="B58" s="56"/>
-      <c r="C58" s="57"/>
-      <c r="D58" s="50"/>
-      <c r="E58" s="51"/>
-      <c r="F58" s="52"/>
-      <c r="G58" s="44"/>
+      <c r="A58" s="53"/>
+      <c r="B58" s="54"/>
+      <c r="C58" s="55"/>
+      <c r="D58" s="48"/>
+      <c r="E58" s="49"/>
+      <c r="F58" s="50"/>
+      <c r="G58" s="42"/>
       <c r="H58" s="11"/>
       <c r="I58" s="11"/>
       <c r="J58" s="11"/>
-      <c r="K58" s="42"/>
+      <c r="K58" s="40"/>
     </row>
     <row r="59" ht="17.25" customHeight="1">
-      <c r="A59" s="55"/>
-      <c r="B59" s="56"/>
-      <c r="C59" s="57"/>
-      <c r="D59" s="50"/>
-      <c r="E59" s="51"/>
-      <c r="F59" s="52"/>
-      <c r="G59" s="44"/>
+      <c r="A59" t="s" s="51">
+        <v>185</v>
+      </c>
+      <c r="B59" t="s" s="52">
+        <v>26</v>
+      </c>
+      <c r="C59" t="s" s="29">
+        <v>186</v>
+      </c>
+      <c r="D59" s="48"/>
+      <c r="E59" s="49"/>
+      <c r="F59" s="50"/>
+      <c r="G59" s="42"/>
       <c r="H59" s="11"/>
       <c r="I59" s="11"/>
       <c r="J59" s="11"/>
-      <c r="K59" s="42"/>
+      <c r="K59" s="40"/>
     </row>
     <row r="60" ht="17.25" customHeight="1">
-      <c r="A60" s="55"/>
-      <c r="B60" s="56"/>
-      <c r="C60" s="57"/>
-      <c r="D60" s="58"/>
-      <c r="E60" s="59"/>
-      <c r="F60" s="60"/>
-      <c r="G60" s="44"/>
+      <c r="A60" t="s" s="51">
+        <v>185</v>
+      </c>
+      <c r="B60" t="s" s="52">
+        <v>30</v>
+      </c>
+      <c r="C60" t="s" s="29">
+        <v>187</v>
+      </c>
+      <c r="D60" s="56"/>
+      <c r="E60" s="57"/>
+      <c r="F60" s="58"/>
+      <c r="G60" s="42"/>
       <c r="H60" s="11"/>
       <c r="I60" s="11"/>
       <c r="J60" s="11"/>
-      <c r="K60" s="42"/>
+      <c r="K60" s="40"/>
     </row>
     <row r="61" ht="18" customHeight="1">
-      <c r="A61" s="61"/>
-      <c r="B61" s="62"/>
-      <c r="C61" s="62"/>
-      <c r="D61" s="37"/>
-      <c r="E61" s="37"/>
-      <c r="F61" s="37"/>
+      <c r="A61" s="59"/>
+      <c r="B61" s="60"/>
+      <c r="C61" s="60"/>
+      <c r="D61" s="35"/>
+      <c r="E61" s="35"/>
+      <c r="F61" s="35"/>
       <c r="G61" s="11"/>
       <c r="H61" s="11"/>
       <c r="I61" s="11"/>
       <c r="J61" s="11"/>
-      <c r="K61" s="42"/>
+      <c r="K61" s="40"/>
     </row>
     <row r="62" ht="18" customHeight="1">
-      <c r="A62" s="44"/>
+      <c r="A62" s="42"/>
       <c r="B62" s="11"/>
       <c r="C62" s="11"/>
       <c r="D62" s="11"/>
@@ -4854,10 +4882,10 @@
       <c r="H62" s="11"/>
       <c r="I62" s="11"/>
       <c r="J62" s="11"/>
-      <c r="K62" s="42"/>
+      <c r="K62" s="40"/>
     </row>
     <row r="63" ht="18" customHeight="1">
-      <c r="A63" s="44"/>
+      <c r="A63" s="42"/>
       <c r="B63" s="11"/>
       <c r="C63" s="11"/>
       <c r="D63" s="11"/>
@@ -4867,10 +4895,10 @@
       <c r="H63" s="11"/>
       <c r="I63" s="11"/>
       <c r="J63" s="11"/>
-      <c r="K63" s="42"/>
+      <c r="K63" s="40"/>
     </row>
     <row r="64" ht="18" customHeight="1">
-      <c r="A64" s="44"/>
+      <c r="A64" s="42"/>
       <c r="B64" s="11"/>
       <c r="C64" s="11"/>
       <c r="D64" s="11"/>
@@ -4880,10 +4908,10 @@
       <c r="H64" s="11"/>
       <c r="I64" s="11"/>
       <c r="J64" s="11"/>
-      <c r="K64" s="42"/>
+      <c r="K64" s="40"/>
     </row>
     <row r="65" ht="18" customHeight="1">
-      <c r="A65" s="44"/>
+      <c r="A65" s="42"/>
       <c r="B65" s="11"/>
       <c r="C65" s="11"/>
       <c r="D65" s="11"/>
@@ -4893,10 +4921,10 @@
       <c r="H65" s="11"/>
       <c r="I65" s="11"/>
       <c r="J65" s="11"/>
-      <c r="K65" s="42"/>
+      <c r="K65" s="40"/>
     </row>
     <row r="66" ht="18" customHeight="1">
-      <c r="A66" s="44"/>
+      <c r="A66" s="42"/>
       <c r="B66" s="11"/>
       <c r="C66" s="11"/>
       <c r="D66" s="11"/>
@@ -4906,10 +4934,10 @@
       <c r="H66" s="11"/>
       <c r="I66" s="11"/>
       <c r="J66" s="11"/>
-      <c r="K66" s="42"/>
+      <c r="K66" s="40"/>
     </row>
     <row r="67" ht="18" customHeight="1">
-      <c r="A67" s="44"/>
+      <c r="A67" s="42"/>
       <c r="B67" s="11"/>
       <c r="C67" s="11"/>
       <c r="D67" s="11"/>
@@ -4919,10 +4947,10 @@
       <c r="H67" s="11"/>
       <c r="I67" s="11"/>
       <c r="J67" s="11"/>
-      <c r="K67" s="42"/>
+      <c r="K67" s="40"/>
     </row>
     <row r="68" ht="18" customHeight="1">
-      <c r="A68" s="44"/>
+      <c r="A68" s="42"/>
       <c r="B68" s="11"/>
       <c r="C68" s="11"/>
       <c r="D68" s="11"/>
@@ -4932,10 +4960,10 @@
       <c r="H68" s="11"/>
       <c r="I68" s="11"/>
       <c r="J68" s="11"/>
-      <c r="K68" s="42"/>
+      <c r="K68" s="40"/>
     </row>
     <row r="69" ht="18" customHeight="1">
-      <c r="A69" s="44"/>
+      <c r="A69" s="42"/>
       <c r="B69" s="11"/>
       <c r="C69" s="11"/>
       <c r="D69" s="11"/>
@@ -4945,20 +4973,20 @@
       <c r="H69" s="11"/>
       <c r="I69" s="11"/>
       <c r="J69" s="11"/>
-      <c r="K69" s="42"/>
+      <c r="K69" s="40"/>
     </row>
     <row r="70" ht="18" customHeight="1">
-      <c r="A70" s="63"/>
-      <c r="B70" s="64"/>
-      <c r="C70" s="64"/>
-      <c r="D70" s="64"/>
-      <c r="E70" s="64"/>
-      <c r="F70" s="64"/>
-      <c r="G70" s="64"/>
-      <c r="H70" s="64"/>
-      <c r="I70" s="64"/>
-      <c r="J70" s="64"/>
-      <c r="K70" s="59"/>
+      <c r="A70" s="61"/>
+      <c r="B70" s="62"/>
+      <c r="C70" s="62"/>
+      <c r="D70" s="62"/>
+      <c r="E70" s="62"/>
+      <c r="F70" s="62"/>
+      <c r="G70" s="62"/>
+      <c r="H70" s="62"/>
+      <c r="I70" s="62"/>
+      <c r="J70" s="62"/>
+      <c r="K70" s="57"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
@@ -4980,161 +5008,161 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.3333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="33.5" style="65" customWidth="1"/>
-    <col min="2" max="2" width="33" style="65" customWidth="1"/>
-    <col min="3" max="3" width="16.3516" style="65" customWidth="1"/>
-    <col min="4" max="4" width="16.3516" style="65" customWidth="1"/>
-    <col min="5" max="5" width="16.3516" style="65" customWidth="1"/>
-    <col min="6" max="6" width="16.3516" style="65" customWidth="1"/>
-    <col min="7" max="7" width="16.3516" style="65" customWidth="1"/>
-    <col min="8" max="8" width="16.3516" style="65" customWidth="1"/>
-    <col min="9" max="9" width="16.3516" style="65" customWidth="1"/>
-    <col min="10" max="10" width="16.3516" style="65" customWidth="1"/>
-    <col min="11" max="256" width="17.3516" style="65" customWidth="1"/>
+    <col min="1" max="1" width="33.5" style="63" customWidth="1"/>
+    <col min="2" max="2" width="33" style="63" customWidth="1"/>
+    <col min="3" max="3" width="16.3516" style="63" customWidth="1"/>
+    <col min="4" max="4" width="16.3516" style="63" customWidth="1"/>
+    <col min="5" max="5" width="16.3516" style="63" customWidth="1"/>
+    <col min="6" max="6" width="16.3516" style="63" customWidth="1"/>
+    <col min="7" max="7" width="16.3516" style="63" customWidth="1"/>
+    <col min="8" max="8" width="16.3516" style="63" customWidth="1"/>
+    <col min="9" max="9" width="16.3516" style="63" customWidth="1"/>
+    <col min="10" max="10" width="16.3516" style="63" customWidth="1"/>
+    <col min="11" max="256" width="17.3516" style="63" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.25" customHeight="1">
-      <c r="A1" s="66"/>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="34"/>
+      <c r="A1" s="64"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="32"/>
     </row>
     <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="67">
-        <v>178</v>
-      </c>
-      <c r="B2" t="s" s="68">
+      <c r="A2" t="s" s="65">
+        <v>188</v>
+      </c>
+      <c r="B2" t="s" s="66">
         <v>14</v>
       </c>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="41"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="39"/>
       <c r="G2" s="11"/>
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
-      <c r="J2" s="42"/>
+      <c r="J2" s="40"/>
     </row>
     <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" t="s" s="31">
-        <v>179</v>
-      </c>
-      <c r="B3" t="s" s="53">
-        <v>180</v>
-      </c>
-      <c r="C3" s="70"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="41"/>
+      <c r="A3" t="s" s="29">
+        <v>189</v>
+      </c>
+      <c r="B3" t="s" s="51">
+        <v>190</v>
+      </c>
+      <c r="C3" s="68"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="39"/>
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
-      <c r="J3" s="42"/>
+      <c r="J3" s="40"/>
     </row>
     <row r="4" ht="20.25" customHeight="1">
-      <c r="A4" s="53"/>
-      <c r="B4" s="72"/>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="41"/>
+      <c r="A4" s="51"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="39"/>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
-      <c r="J4" s="42"/>
+      <c r="J4" s="40"/>
     </row>
     <row r="5" ht="20.25" customHeight="1">
-      <c r="A5" s="53"/>
-      <c r="B5" s="72"/>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="41"/>
+      <c r="A5" s="51"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="39"/>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
       <c r="I5" s="11"/>
-      <c r="J5" s="42"/>
+      <c r="J5" s="40"/>
     </row>
     <row r="6" ht="20.25" customHeight="1">
-      <c r="A6" s="53"/>
-      <c r="B6" s="70"/>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="41"/>
+      <c r="A6" s="51"/>
+      <c r="B6" s="68"/>
+      <c r="C6" s="69"/>
+      <c r="D6" s="69"/>
+      <c r="E6" s="69"/>
+      <c r="F6" s="39"/>
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
-      <c r="J6" s="42"/>
+      <c r="J6" s="40"/>
     </row>
     <row r="7" ht="20.25" customHeight="1">
-      <c r="A7" s="53"/>
-      <c r="B7" s="70"/>
-      <c r="C7" s="71"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="41"/>
+      <c r="A7" s="51"/>
+      <c r="B7" s="68"/>
+      <c r="C7" s="69"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="39"/>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
-      <c r="J7" s="42"/>
+      <c r="J7" s="40"/>
     </row>
     <row r="8" ht="20.25" customHeight="1">
-      <c r="A8" s="53"/>
-      <c r="B8" s="70"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="71"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="41"/>
+      <c r="A8" s="51"/>
+      <c r="B8" s="68"/>
+      <c r="C8" s="69"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="69"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
-      <c r="J8" s="42"/>
+      <c r="J8" s="40"/>
     </row>
     <row r="9" ht="20.25" customHeight="1">
-      <c r="A9" s="53"/>
-      <c r="B9" s="70"/>
-      <c r="C9" s="71"/>
-      <c r="D9" s="71"/>
-      <c r="E9" s="71"/>
-      <c r="F9" s="41"/>
+      <c r="A9" s="51"/>
+      <c r="B9" s="68"/>
+      <c r="C9" s="69"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="69"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
-      <c r="J9" s="42"/>
+      <c r="J9" s="40"/>
     </row>
     <row r="10" ht="20.25" customHeight="1">
-      <c r="A10" s="53"/>
-      <c r="B10" s="70"/>
-      <c r="C10" s="71"/>
-      <c r="D10" s="71"/>
-      <c r="E10" s="71"/>
-      <c r="F10" s="41"/>
+      <c r="A10" s="51"/>
+      <c r="B10" s="68"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
-      <c r="J10" s="42"/>
+      <c r="J10" s="40"/>
     </row>
     <row r="11" ht="18" customHeight="1">
-      <c r="A11" s="61"/>
-      <c r="B11" s="62"/>
-      <c r="C11" s="62"/>
-      <c r="D11" s="62"/>
-      <c r="E11" s="62"/>
+      <c r="A11" s="59"/>
+      <c r="B11" s="60"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="60"/>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
       <c r="I11" s="11"/>
-      <c r="J11" s="42"/>
+      <c r="J11" s="40"/>
     </row>
     <row r="12" ht="18" customHeight="1">
-      <c r="A12" s="44"/>
+      <c r="A12" s="42"/>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
@@ -5143,10 +5171,10 @@
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
       <c r="I12" s="11"/>
-      <c r="J12" s="42"/>
+      <c r="J12" s="40"/>
     </row>
     <row r="13" ht="18" customHeight="1">
-      <c r="A13" s="44"/>
+      <c r="A13" s="42"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
@@ -5155,10 +5183,10 @@
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
       <c r="I13" s="11"/>
-      <c r="J13" s="42"/>
+      <c r="J13" s="40"/>
     </row>
     <row r="14" ht="18" customHeight="1">
-      <c r="A14" s="44"/>
+      <c r="A14" s="42"/>
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
@@ -5167,10 +5195,10 @@
       <c r="G14" s="11"/>
       <c r="H14" s="11"/>
       <c r="I14" s="11"/>
-      <c r="J14" s="42"/>
+      <c r="J14" s="40"/>
     </row>
     <row r="15" ht="18" customHeight="1">
-      <c r="A15" s="44"/>
+      <c r="A15" s="42"/>
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
@@ -5179,10 +5207,10 @@
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
-      <c r="J15" s="42"/>
+      <c r="J15" s="40"/>
     </row>
     <row r="16" ht="18" customHeight="1">
-      <c r="A16" s="44"/>
+      <c r="A16" s="42"/>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
@@ -5191,10 +5219,10 @@
       <c r="G16" s="11"/>
       <c r="H16" s="11"/>
       <c r="I16" s="11"/>
-      <c r="J16" s="42"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" ht="18" customHeight="1">
-      <c r="A17" s="44"/>
+      <c r="A17" s="42"/>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
@@ -5203,10 +5231,10 @@
       <c r="G17" s="11"/>
       <c r="H17" s="11"/>
       <c r="I17" s="11"/>
-      <c r="J17" s="42"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" ht="18" customHeight="1">
-      <c r="A18" s="44"/>
+      <c r="A18" s="42"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
@@ -5215,10 +5243,10 @@
       <c r="G18" s="11"/>
       <c r="H18" s="11"/>
       <c r="I18" s="11"/>
-      <c r="J18" s="42"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" ht="18" customHeight="1">
-      <c r="A19" s="44"/>
+      <c r="A19" s="42"/>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
@@ -5227,19 +5255,19 @@
       <c r="G19" s="11"/>
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
-      <c r="J19" s="42"/>
+      <c r="J19" s="40"/>
     </row>
     <row r="20" ht="18" customHeight="1">
-      <c r="A20" s="63"/>
-      <c r="B20" s="64"/>
-      <c r="C20" s="64"/>
-      <c r="D20" s="64"/>
-      <c r="E20" s="64"/>
-      <c r="F20" s="64"/>
-      <c r="G20" s="64"/>
-      <c r="H20" s="64"/>
-      <c r="I20" s="64"/>
-      <c r="J20" s="59"/>
+      <c r="A20" s="61"/>
+      <c r="B20" s="62"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="62"/>
+      <c r="E20" s="62"/>
+      <c r="F20" s="62"/>
+      <c r="G20" s="62"/>
+      <c r="H20" s="62"/>
+      <c r="I20" s="62"/>
+      <c r="J20" s="57"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>